<commit_message>
Added test for declined cards.
</commit_message>
<xml_diff>
--- a/data/tickets.xlsx
+++ b/data/tickets.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Successful" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Declined" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="183">
   <si>
     <t>id_testdata</t>
   </si>
@@ -441,9 +441,6 @@
     <t>4000004840000008</t>
   </si>
   <si>
-    <t>22223</t>
-  </si>
-  <si>
     <t>Tom</t>
   </si>
   <si>
@@ -456,10 +453,118 @@
     <t>SE23 1PJ</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>2:00 PM CT</t>
+    <t>declined_card_number</t>
+  </si>
+  <si>
+    <t>GoDo-485</t>
+  </si>
+  <si>
+    <t>GoDo-486</t>
+  </si>
+  <si>
+    <t>GoDo-487</t>
+  </si>
+  <si>
+    <t>GoDo-488</t>
+  </si>
+  <si>
+    <t>GoDo-489</t>
+  </si>
+  <si>
+    <t>godo-485@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-486@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-487@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-488@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-489@mailinator.com</t>
+  </si>
+  <si>
+    <t>4000000000000002</t>
+  </si>
+  <si>
+    <t>4000000000000077</t>
+  </si>
+  <si>
+    <t>4100000000000019</t>
+  </si>
+  <si>
+    <t>4000000000000093</t>
+  </si>
+  <si>
+    <t>4000000000000127</t>
+  </si>
+  <si>
+    <t>4000000000000028</t>
+  </si>
+  <si>
+    <t>4000000000000069</t>
+  </si>
+  <si>
+    <t>4000000000000044</t>
+  </si>
+  <si>
+    <t>4000000000000119</t>
+  </si>
+  <si>
+    <t>4000000000009235</t>
+  </si>
+  <si>
+    <t>GoDo-696</t>
+  </si>
+  <si>
+    <t>godo-696@mailinator.com</t>
+  </si>
+  <si>
+    <t>GoDo-697</t>
+  </si>
+  <si>
+    <t>GoDo-698</t>
+  </si>
+  <si>
+    <t>GoDo-699</t>
+  </si>
+  <si>
+    <t>GoDo-700</t>
+  </si>
+  <si>
+    <t>4000000000000010</t>
+  </si>
+  <si>
+    <t>4000000000000036</t>
+  </si>
+  <si>
+    <t>4000000000000101</t>
+  </si>
+  <si>
+    <t>4000000000000341</t>
+  </si>
+  <si>
+    <t>4000000000003063</t>
+  </si>
+  <si>
+    <t>5105105105105100 </t>
+  </si>
+  <si>
+    <t>godo-698@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-697@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-700@mailinator.com</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7:30 PM CT</t>
   </si>
 </sst>
 </file>
@@ -811,9 +916,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,10 +1092,10 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>64</v>
@@ -1067,10 +1172,10 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>39</v>
@@ -1147,10 +1252,10 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>92</v>
@@ -1227,10 +1332,10 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>95</v>
@@ -1258,9 +1363,6 @@
       </c>
       <c r="AA5" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="AD5" s="1" t="s">
         <v>46</v>
@@ -1307,10 +1409,10 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>98</v>
@@ -1387,10 +1489,10 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>101</v>
@@ -1467,10 +1569,10 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>114</v>
@@ -1547,10 +1649,10 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>108</v>
@@ -1627,10 +1729,10 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>112</v>
@@ -1707,10 +1809,10 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>118</v>
@@ -1738,9 +1840,6 @@
       </c>
       <c r="AA11" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="AD11" s="1" t="s">
         <v>90</v>
@@ -1787,10 +1886,10 @@
         <v>5</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>122</v>
@@ -1818,9 +1917,6 @@
       </c>
       <c r="AA12" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="AD12" s="1" t="s">
         <v>90</v>
@@ -1867,10 +1963,10 @@
         <v>5</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>126</v>
@@ -1947,10 +2043,10 @@
         <v>5</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>134</v>
@@ -1978,9 +2074,6 @@
       </c>
       <c r="AA14" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="AB14" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="AD14" s="1" t="s">
         <v>90</v>
@@ -2027,10 +2120,10 @@
         <v>5</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>128</v>
@@ -2107,10 +2200,10 @@
         <v>5</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>138</v>
@@ -2138,9 +2231,6 @@
       </c>
       <c r="AA16" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="AB16" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="AD16" s="1" t="s">
         <v>90</v>
@@ -2187,16 +2277,16 @@
         <v>5</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="P17" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q17" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="R17" s="1">
         <v>15044466025</v>
@@ -2211,7 +2301,7 @@
         <v>42</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Z17" s="1" t="s">
         <v>44</v>
@@ -2220,7 +2310,7 @@
         <v>45</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AD17" s="1" t="s">
         <v>90</v>
@@ -2249,13 +2339,1014 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD22" sqref="AD22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" style="1" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="13.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="20.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="38.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="18.85546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="20.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="23.7109375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="22.140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="12.85546875" style="1" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11" style="1" customWidth="1"/>
+    <col min="30" max="30" width="14.140625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="13.28515625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="10.5703125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="15" style="1" customWidth="1"/>
+    <col min="34" max="34" width="13.7109375" style="1" customWidth="1"/>
+    <col min="35" max="35" width="15" style="1" customWidth="1"/>
+    <col min="36" max="36" width="15.42578125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="18" style="1" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M2" s="1">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R2" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S2" t="s">
+        <v>151</v>
+      </c>
+      <c r="T2" s="1">
+        <v>35801</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>35801</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S3" t="s">
+        <v>152</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R4" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S4" t="s">
+        <v>153</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R5" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S5" t="s">
+        <v>154</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R6" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S6" t="s">
+        <v>155</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M7" s="1">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R7" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S7" t="s">
+        <v>167</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M8" s="1">
+        <v>5</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="R8" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S8" t="s">
+        <v>179</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R9" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S9" t="s">
+        <v>178</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R10" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S10" t="s">
+        <v>178</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>35801</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M11" s="1">
+        <v>5</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="R11" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S11" t="s">
+        <v>180</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S12"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S13"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S14"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S15"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S16"/>
+    </row>
+    <row r="17" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S17"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added new test for customer-facing(all valid cards)
</commit_message>
<xml_diff>
--- a/data/tickets.xlsx
+++ b/data/tickets.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Successful" sheetId="1" r:id="rId1"/>
     <sheet name="Declined" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Customer Successful" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="235">
   <si>
     <t>id_testdata</t>
   </si>
@@ -564,10 +564,163 @@
     <t>4:15 PM CT</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>5:10 AM CT</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>godo-473_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-474_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-475_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-476_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-477_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-478_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-american_express_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-479_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-discover_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-480_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-diners_club_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-481_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-unionpay_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-482_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-483_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-484_cus@mailinator.com</t>
+  </si>
+  <si>
+    <t>GoDo-473-c</t>
+  </si>
+  <si>
+    <t>GoDo-474-c</t>
+  </si>
+  <si>
+    <t>GoDo-475-c</t>
+  </si>
+  <si>
+    <t>GoDo-476-c</t>
+  </si>
+  <si>
+    <t>GoDo-477-c</t>
+  </si>
+  <si>
+    <t>GoDo-478-c</t>
+  </si>
+  <si>
+    <t>GoDo-American Express-c</t>
+  </si>
+  <si>
+    <t>GoDo-479-c</t>
+  </si>
+  <si>
+    <t>GoDo-Discover-c</t>
+  </si>
+  <si>
+    <t>GoDo-480-c</t>
+  </si>
+  <si>
+    <t>GoDo-Diners Club-c</t>
+  </si>
+  <si>
+    <t>GoDo-481-c</t>
+  </si>
+  <si>
+    <t>GoDo-UnionPay-c</t>
+  </si>
+  <si>
+    <t>GoDo-482-c</t>
+  </si>
+  <si>
+    <t>GoDo-483-c</t>
+  </si>
+  <si>
+    <t>GoDo-484-c</t>
+  </si>
+  <si>
+    <t>https://dev.godo.io/customer_facing.aspx?Activity=b5382243-b660-451f-a2e0-c9a99dac7045</t>
+  </si>
+  <si>
+    <t>AlertTest</t>
+  </si>
+  <si>
+    <t>Senior</t>
+  </si>
+  <si>
+    <t>100.00</t>
+  </si>
+  <si>
+    <t>111.00</t>
+  </si>
+  <si>
+    <t>5.00</t>
+  </si>
+  <si>
+    <t>6.00</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>50.00</t>
+  </si>
+  <si>
+    <t>2.50</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>20.00</t>
+  </si>
+  <si>
+    <t>22.20</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>1.20</t>
+  </si>
+  <si>
+    <t>05:00 AM</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>55.50</t>
   </si>
 </sst>
 </file>
@@ -919,14 +1072,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O20" sqref="O20"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
@@ -1091,11 +1244,11 @@
       <c r="L2" s="1">
         <v>2018</v>
       </c>
-      <c r="M2" s="1">
-        <v>5</v>
+      <c r="M2" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>181</v>
@@ -1175,7 +1328,7 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>181</v>
@@ -1255,7 +1408,7 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>181</v>
@@ -1335,7 +1488,7 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>181</v>
@@ -1412,7 +1565,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>181</v>
@@ -1492,7 +1645,7 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>181</v>
@@ -1572,7 +1725,7 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>181</v>
@@ -1652,7 +1805,7 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>181</v>
@@ -1732,7 +1885,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>181</v>
@@ -1812,7 +1965,7 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>181</v>
@@ -1889,7 +2042,7 @@
         <v>5</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>181</v>
@@ -1966,7 +2119,7 @@
         <v>5</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>181</v>
@@ -2046,7 +2199,7 @@
         <v>5</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>181</v>
@@ -2123,7 +2276,7 @@
         <v>5</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>181</v>
@@ -2203,7 +2356,7 @@
         <v>5</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>181</v>
@@ -2280,7 +2433,7 @@
         <v>5</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>181</v>
@@ -2345,8 +2498,8 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P15" sqref="P15"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2528,7 +2681,7 @@
         <v>182</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>63</v>
@@ -2611,7 +2764,7 @@
         <v>182</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>38</v>
@@ -2694,7 +2847,7 @@
         <v>182</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>91</v>
@@ -2777,7 +2930,7 @@
         <v>182</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>94</v>
@@ -2860,7 +3013,7 @@
         <v>182</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>97</v>
@@ -2943,7 +3096,7 @@
         <v>182</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>100</v>
@@ -3026,7 +3179,7 @@
         <v>182</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>113</v>
@@ -3109,7 +3262,7 @@
         <v>182</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>107</v>
@@ -3192,7 +3345,7 @@
         <v>182</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>111</v>
@@ -3275,7 +3428,7 @@
         <v>182</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>117</v>
@@ -3355,12 +3508,1413 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH9" sqref="AH9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" style="1" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="13.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="20.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="38.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="18.85546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="20.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="20" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.85546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="11" style="1" customWidth="1"/>
+    <col min="28" max="28" width="13.28515625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="13.7109375" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15" style="1" customWidth="1"/>
+    <col min="32" max="32" width="15.42578125" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L2" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M2" s="1">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="R2" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S2" t="s">
+        <v>190</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R3" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S3" t="s">
+        <v>191</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="R4" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S4" t="s">
+        <v>192</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>35801</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="R5" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S5" t="s">
+        <v>193</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>35801</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="R6" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S6" t="s">
+        <v>194</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L7" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M7" s="1">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="R7" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S7" t="s">
+        <v>195</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L8" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M8" s="1">
+        <v>5</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="R8" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S8" t="s">
+        <v>196</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L9" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="R9" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S9" t="s">
+        <v>197</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L10" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R10" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S10" t="s">
+        <v>198</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L11" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M11" s="1">
+        <v>5</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="R11" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S11" t="s">
+        <v>199</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L12" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M12" s="1">
+        <v>5</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="R12" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S12" t="s">
+        <v>200</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L13" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R13" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S13" t="s">
+        <v>185</v>
+      </c>
+      <c r="T13" s="1">
+        <v>35801</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>35801</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L14" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M14" s="1">
+        <v>5</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R14" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S14" t="s">
+        <v>186</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L15" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M15" s="1">
+        <v>5</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="R15" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S15" t="s">
+        <v>187</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AF15" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L16" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M16" s="1">
+        <v>5</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R16" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S16" t="s">
+        <v>188</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L17" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M17" s="1">
+        <v>5</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R17" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S17" t="s">
+        <v>189</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC17" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AF17" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added test for customer-facing (invalid credit cards)
</commit_message>
<xml_diff>
--- a/data/tickets.xlsx
+++ b/data/tickets.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Successful" sheetId="1" r:id="rId1"/>
     <sheet name="Declined" sheetId="2" r:id="rId2"/>
-    <sheet name="Customer Successful" sheetId="3" r:id="rId3"/>
+    <sheet name="Customer Successful" sheetId="4" r:id="rId3"/>
+    <sheet name="Customer Declined" sheetId="5" r:id="rId4"/>
+    <sheet name="Customer Successful--" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="253">
   <si>
     <t>id_testdata</t>
   </si>
@@ -717,10 +719,64 @@
     <t>05:00 AM</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>55.50</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>https://dev.godo.io/customer_facing.aspx?Activity=b7308051-c34a-469e-a283-db155f09a879</t>
+  </si>
+  <si>
+    <t>Super Test Activity</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>02:30 PM</t>
+  </si>
+  <si>
+    <t>116.00</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>GoDo-701</t>
+  </si>
+  <si>
+    <t>GoDo-702</t>
+  </si>
+  <si>
+    <t>GoDo-703</t>
+  </si>
+  <si>
+    <t>GoDo-704</t>
+  </si>
+  <si>
+    <t>GoDo-705</t>
+  </si>
+  <si>
+    <t>GoDo-706</t>
+  </si>
+  <si>
+    <t>4000000000003055</t>
+  </si>
+  <si>
+    <t>GoDo-707</t>
+  </si>
+  <si>
+    <t>GoDo-708</t>
+  </si>
+  <si>
+    <t>GoDo-709</t>
+  </si>
+  <si>
+    <t>GoDo-710</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -745,12 +801,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -765,10 +827,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1073,7 +1136,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -3508,11 +3571,2238 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="13.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="38.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="20" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11" style="1" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15" style="1" customWidth="1"/>
+    <col min="24" max="24" width="15.42578125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M2" t="s">
+        <v>190</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L3" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M3" t="s">
+        <v>191</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L4" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M4" t="s">
+        <v>192</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="1">
+        <v>35801</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L5" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M5" t="s">
+        <v>193</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="1">
+        <v>35801</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M6" t="s">
+        <v>194</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M7" t="s">
+        <v>195</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G8" s="1">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L8" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M8" t="s">
+        <v>196</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G9" s="1">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L9" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M9" t="s">
+        <v>197</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G10" s="1">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L10" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M10" t="s">
+        <v>198</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G11" s="1">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L11" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M11" t="s">
+        <v>199</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G12" s="1">
+        <v>5</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L12" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M12" t="s">
+        <v>200</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M13" t="s">
+        <v>185</v>
+      </c>
+      <c r="N13" s="1">
+        <v>35801</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S13" s="1">
+        <v>35801</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G14" s="1">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M14" t="s">
+        <v>186</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G15" s="1">
+        <v>5</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M15" t="s">
+        <v>187</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L16" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M16" t="s">
+        <v>188</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G17" s="1">
+        <v>5</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L17" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="M17" t="s">
+        <v>189</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="58" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" style="1" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="13.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="20.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="38.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="18.85546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="20.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="23.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="22.140625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="11" style="1" customWidth="1"/>
+    <col min="29" max="29" width="13.28515625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5703125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15" style="1" customWidth="1"/>
+    <col min="32" max="32" width="13.7109375" style="1" customWidth="1"/>
+    <col min="33" max="33" width="15" style="1" customWidth="1"/>
+    <col min="34" max="34" width="15.42578125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="18" style="1" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L2" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M2" s="1">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R2" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S2" t="s">
+        <v>150</v>
+      </c>
+      <c r="T2" s="1">
+        <v>35801</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>35801</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S3" t="s">
+        <v>151</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="R4" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S4" t="s">
+        <v>152</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R5" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S5" t="s">
+        <v>153</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R6" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S6" t="s">
+        <v>154</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L7" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M7" s="1">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="R7" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S7" t="s">
+        <v>166</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L8" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M8" s="1">
+        <v>5</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R8" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S8" t="s">
+        <v>178</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L9" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="R9" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S9" t="s">
+        <v>177</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L10" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="R10" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S10" t="s">
+        <v>177</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>35801</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L11" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M11" s="1">
+        <v>5</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="R11" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S11" t="s">
+        <v>179</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="S12"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="S13"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="S14"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="S15"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="S16"/>
+    </row>
+    <row r="17" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH9" sqref="AH9"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3677,7 +5967,7 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>232</v>
@@ -3725,7 +6015,7 @@
         <v>227</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -3757,7 +6047,7 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>232</v>
@@ -3805,7 +6095,7 @@
         <v>227</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -3837,7 +6127,7 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>232</v>
@@ -3885,7 +6175,7 @@
         <v>227</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -3917,7 +6207,7 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>232</v>
@@ -3965,7 +6255,7 @@
         <v>227</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
@@ -3997,7 +6287,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>232</v>
@@ -4042,7 +6332,7 @@
         <v>227</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -4074,7 +6364,7 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>232</v>
@@ -4151,7 +6441,7 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>232</v>
@@ -4231,7 +6521,7 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>232</v>
@@ -4308,7 +6598,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>232</v>
@@ -4388,7 +6678,7 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>232</v>
@@ -4465,7 +6755,7 @@
         <v>5</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>232</v>
@@ -4545,7 +6835,7 @@
         <v>184</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>232</v>
@@ -4625,7 +6915,7 @@
         <v>5</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>232</v>
@@ -4705,7 +6995,7 @@
         <v>5</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>232</v>
@@ -4785,7 +7075,7 @@
         <v>5</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>232</v>
@@ -4862,7 +7152,7 @@
         <v>5</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
Test data was updated.
</commit_message>
<xml_diff>
--- a/data/tickets.xlsx
+++ b/data/tickets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Successful" sheetId="1" r:id="rId1"/>
@@ -569,9 +569,6 @@
     <t>10</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -777,6 +774,9 @@
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1137,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G26" sqref="G26"/>
+      <selection pane="topRight" activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,10 +1308,10 @@
         <v>2018</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>181</v>
@@ -1391,7 +1391,7 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>181</v>
@@ -1471,7 +1471,7 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>181</v>
@@ -1551,7 +1551,7 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>181</v>
@@ -1628,7 +1628,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>181</v>
@@ -1708,7 +1708,7 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>181</v>
@@ -1788,7 +1788,7 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>181</v>
@@ -1868,7 +1868,7 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>181</v>
@@ -1948,7 +1948,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>181</v>
@@ -2028,7 +2028,7 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>181</v>
@@ -2105,7 +2105,7 @@
         <v>5</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>181</v>
@@ -2182,7 +2182,7 @@
         <v>5</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>181</v>
@@ -2262,7 +2262,7 @@
         <v>5</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>181</v>
@@ -2339,7 +2339,7 @@
         <v>5</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>181</v>
@@ -2419,7 +2419,7 @@
         <v>5</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>181</v>
@@ -2496,7 +2496,7 @@
         <v>5</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>181</v>
@@ -2561,7 +2561,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
@@ -3575,7 +3575,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H21" sqref="H21"/>
+      <selection pane="topRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3681,19 +3681,19 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F2" s="1">
         <v>2018</v>
@@ -3702,10 +3702,10 @@
         <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>100</v>
@@ -3717,7 +3717,7 @@
         <v>15044466025</v>
       </c>
       <c r="M2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>80</v>
@@ -3738,36 +3738,36 @@
         <v>80</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F3" s="1">
         <v>2018</v>
@@ -3776,10 +3776,10 @@
         <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>113</v>
@@ -3791,7 +3791,7 @@
         <v>15044466025</v>
       </c>
       <c r="M3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>80</v>
@@ -3812,36 +3812,36 @@
         <v>80</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F4" s="1">
         <v>2018</v>
@@ -3850,10 +3850,10 @@
         <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>107</v>
@@ -3865,7 +3865,7 @@
         <v>15044466025</v>
       </c>
       <c r="M4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>81</v>
@@ -3886,36 +3886,36 @@
         <v>35801</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F5" s="1">
         <v>2018</v>
@@ -3924,10 +3924,10 @@
         <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>111</v>
@@ -3939,7 +3939,7 @@
         <v>15044466025</v>
       </c>
       <c r="M5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>81</v>
@@ -3960,36 +3960,36 @@
         <v>35801</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F6" s="1">
         <v>2018</v>
@@ -3998,10 +3998,10 @@
         <v>5</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>117</v>
@@ -4013,7 +4013,7 @@
         <v>15044466025</v>
       </c>
       <c r="M6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>82</v>
@@ -4031,36 +4031,36 @@
         <v>44</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F7" s="1">
         <v>2018</v>
@@ -4069,10 +4069,10 @@
         <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>121</v>
@@ -4084,7 +4084,7 @@
         <v>15044466025</v>
       </c>
       <c r="M7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>82</v>
@@ -4102,36 +4102,36 @@
         <v>44</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F8" s="1">
         <v>2018</v>
@@ -4140,10 +4140,10 @@
         <v>5</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>125</v>
@@ -4155,7 +4155,7 @@
         <v>15044466025</v>
       </c>
       <c r="M8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>83</v>
@@ -4176,36 +4176,36 @@
         <v>83</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F9" s="1">
         <v>2018</v>
@@ -4214,10 +4214,10 @@
         <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>133</v>
@@ -4229,7 +4229,7 @@
         <v>15044466025</v>
       </c>
       <c r="M9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>85</v>
@@ -4247,36 +4247,36 @@
         <v>44</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F10" s="1">
         <v>2018</v>
@@ -4285,10 +4285,10 @@
         <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>127</v>
@@ -4300,7 +4300,7 @@
         <v>15044466025</v>
       </c>
       <c r="M10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>84</v>
@@ -4321,36 +4321,36 @@
         <v>136</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F11" s="1">
         <v>2018</v>
@@ -4359,10 +4359,10 @@
         <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>137</v>
@@ -4374,7 +4374,7 @@
         <v>15044466025</v>
       </c>
       <c r="M11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>85</v>
@@ -4392,36 +4392,36 @@
         <v>44</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F12" s="1">
         <v>2018</v>
@@ -4430,10 +4430,10 @@
         <v>5</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>140</v>
@@ -4445,7 +4445,7 @@
         <v>15044466025</v>
       </c>
       <c r="M12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>86</v>
@@ -4466,48 +4466,48 @@
         <v>143</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F13" s="1">
         <v>2018</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>63</v>
@@ -4519,7 +4519,7 @@
         <v>15044466025</v>
       </c>
       <c r="M13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N13" s="1">
         <v>35801</v>
@@ -4540,36 +4540,36 @@
         <v>35801</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F14" s="1">
         <v>2018</v>
@@ -4578,10 +4578,10 @@
         <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>38</v>
@@ -4593,7 +4593,7 @@
         <v>15044466025</v>
       </c>
       <c r="M14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>76</v>
@@ -4614,36 +4614,36 @@
         <v>76</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F15" s="1">
         <v>2018</v>
@@ -4652,10 +4652,10 @@
         <v>5</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>91</v>
@@ -4667,7 +4667,7 @@
         <v>15044466025</v>
       </c>
       <c r="M15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>77</v>
@@ -4688,36 +4688,36 @@
         <v>77</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F16" s="1">
         <v>2018</v>
@@ -4726,10 +4726,10 @@
         <v>5</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>94</v>
@@ -4741,7 +4741,7 @@
         <v>15044466025</v>
       </c>
       <c r="M16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>78</v>
@@ -4759,36 +4759,36 @@
         <v>44</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F17" s="1">
         <v>2018</v>
@@ -4797,10 +4797,10 @@
         <v>5</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>97</v>
@@ -4812,7 +4812,7 @@
         <v>15044466025</v>
       </c>
       <c r="M17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>79</v>
@@ -4833,19 +4833,19 @@
         <v>79</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -4858,9 +4858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O15" sqref="O15"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5004,19 +5004,19 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L2" s="1">
         <v>2018</v>
@@ -5025,10 +5025,10 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>63</v>
@@ -5064,36 +5064,36 @@
         <v>35801</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L3" s="1">
         <v>2018</v>
@@ -5102,10 +5102,10 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>38</v>
@@ -5141,36 +5141,36 @@
         <v>76</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L4" s="1">
         <v>2018</v>
@@ -5179,10 +5179,10 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>91</v>
@@ -5218,36 +5218,36 @@
         <v>77</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L5" s="1">
         <v>2018</v>
@@ -5256,10 +5256,10 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>94</v>
@@ -5295,36 +5295,36 @@
         <v>78</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L6" s="1">
         <v>2018</v>
@@ -5333,10 +5333,10 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>97</v>
@@ -5372,36 +5372,36 @@
         <v>79</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L7" s="1">
         <v>2018</v>
@@ -5410,10 +5410,10 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>100</v>
@@ -5434,7 +5434,7 @@
         <v>41</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>157</v>
@@ -5449,36 +5449,36 @@
         <v>80</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L8" s="1">
         <v>2018</v>
@@ -5487,10 +5487,10 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>113</v>
@@ -5526,36 +5526,36 @@
         <v>80</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF8" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L9" s="1">
         <v>2018</v>
@@ -5564,10 +5564,10 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>107</v>
@@ -5603,36 +5603,36 @@
         <v>80</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE9" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF9" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AG9" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L10" s="1">
         <v>2018</v>
@@ -5641,10 +5641,10 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>111</v>
@@ -5680,36 +5680,36 @@
         <v>35801</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AG10" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L11" s="1">
         <v>2018</v>
@@ -5718,10 +5718,10 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>117</v>
@@ -5757,19 +5757,19 @@
         <v>76</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF11" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
@@ -5798,11 +5798,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF17"/>
+  <dimension ref="A1:AF45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5940,13 +5940,13 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>61</v>
@@ -5958,7 +5958,7 @@
         <v>37</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L2" s="1">
         <v>2018</v>
@@ -5967,10 +5967,10 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>100</v>
@@ -5982,7 +5982,7 @@
         <v>15044466025</v>
       </c>
       <c r="S2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>80</v>
@@ -6003,30 +6003,30 @@
         <v>80</v>
       </c>
       <c r="AB2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AC2" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="AF2" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>61</v>
@@ -6038,7 +6038,7 @@
         <v>37</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L3" s="1">
         <v>2018</v>
@@ -6047,10 +6047,10 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>113</v>
@@ -6062,7 +6062,7 @@
         <v>15044466025</v>
       </c>
       <c r="S3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>80</v>
@@ -6083,30 +6083,30 @@
         <v>80</v>
       </c>
       <c r="AB3" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AC3" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="AE3" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="AF3" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>61</v>
@@ -6118,7 +6118,7 @@
         <v>37</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L4" s="1">
         <v>2018</v>
@@ -6127,10 +6127,10 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>107</v>
@@ -6142,7 +6142,7 @@
         <v>15044466025</v>
       </c>
       <c r="S4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>81</v>
@@ -6163,30 +6163,30 @@
         <v>35801</v>
       </c>
       <c r="AB4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD4" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AC4" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="AE4" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="AF4" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>61</v>
@@ -6198,7 +6198,7 @@
         <v>37</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L5" s="1">
         <v>2018</v>
@@ -6207,10 +6207,10 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>111</v>
@@ -6222,7 +6222,7 @@
         <v>15044466025</v>
       </c>
       <c r="S5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>81</v>
@@ -6243,30 +6243,30 @@
         <v>35801</v>
       </c>
       <c r="AB5" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD5" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AC5" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="AE5" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="AF5" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>61</v>
@@ -6278,7 +6278,7 @@
         <v>37</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L6" s="1">
         <v>2018</v>
@@ -6287,10 +6287,10 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>117</v>
@@ -6302,7 +6302,7 @@
         <v>15044466025</v>
       </c>
       <c r="S6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>82</v>
@@ -6320,30 +6320,30 @@
         <v>44</v>
       </c>
       <c r="AB6" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD6" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AC6" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AE6" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="AE6" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="AF6" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>61</v>
@@ -6355,7 +6355,7 @@
         <v>37</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L7" s="1">
         <v>2018</v>
@@ -6364,10 +6364,10 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>121</v>
@@ -6379,7 +6379,7 @@
         <v>15044466025</v>
       </c>
       <c r="S7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>82</v>
@@ -6397,30 +6397,30 @@
         <v>44</v>
       </c>
       <c r="AB7" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AF7" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE7" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="AF7" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>61</v>
@@ -6432,7 +6432,7 @@
         <v>37</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L8" s="1">
         <v>2018</v>
@@ -6441,10 +6441,10 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>125</v>
@@ -6456,7 +6456,7 @@
         <v>15044466025</v>
       </c>
       <c r="S8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>83</v>
@@ -6477,30 +6477,30 @@
         <v>83</v>
       </c>
       <c r="AB8" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AF8" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE8" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="AF8" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>61</v>
@@ -6512,7 +6512,7 @@
         <v>37</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L9" s="1">
         <v>2018</v>
@@ -6521,10 +6521,10 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>133</v>
@@ -6536,7 +6536,7 @@
         <v>15044466025</v>
       </c>
       <c r="S9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>85</v>
@@ -6554,30 +6554,30 @@
         <v>44</v>
       </c>
       <c r="AB9" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AF9" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD9" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE9" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="AF9" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>61</v>
@@ -6589,7 +6589,7 @@
         <v>37</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L10" s="1">
         <v>2018</v>
@@ -6598,10 +6598,10 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>127</v>
@@ -6613,7 +6613,7 @@
         <v>15044466025</v>
       </c>
       <c r="S10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>84</v>
@@ -6634,30 +6634,30 @@
         <v>136</v>
       </c>
       <c r="AB10" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AF10" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="AC10" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD10" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE10" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="AF10" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>61</v>
@@ -6669,7 +6669,7 @@
         <v>37</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L11" s="1">
         <v>2018</v>
@@ -6678,10 +6678,10 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>137</v>
@@ -6693,7 +6693,7 @@
         <v>15044466025</v>
       </c>
       <c r="S11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>85</v>
@@ -6711,30 +6711,30 @@
         <v>44</v>
       </c>
       <c r="AB11" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AF11" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD11" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE11" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="AF11" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>61</v>
@@ -6746,7 +6746,7 @@
         <v>37</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L12" s="1">
         <v>2018</v>
@@ -6755,10 +6755,10 @@
         <v>5</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>140</v>
@@ -6770,7 +6770,7 @@
         <v>15044466025</v>
       </c>
       <c r="S12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>86</v>
@@ -6791,30 +6791,30 @@
         <v>143</v>
       </c>
       <c r="AB12" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AF12" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE12" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="AF12" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -6826,19 +6826,19 @@
         <v>37</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L13" s="1">
         <v>2018</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>63</v>
@@ -6850,7 +6850,7 @@
         <v>15044466025</v>
       </c>
       <c r="S13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="T13" s="1">
         <v>35801</v>
@@ -6871,30 +6871,30 @@
         <v>35801</v>
       </c>
       <c r="AB13" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF13" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AE13" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AF13" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -6906,7 +6906,7 @@
         <v>37</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L14" s="1">
         <v>2018</v>
@@ -6915,10 +6915,10 @@
         <v>5</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>38</v>
@@ -6930,7 +6930,7 @@
         <v>15044466025</v>
       </c>
       <c r="S14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T14" s="1" t="s">
         <v>76</v>
@@ -6951,30 +6951,30 @@
         <v>76</v>
       </c>
       <c r="AB14" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF14" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD14" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AE14" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AF14" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -6986,7 +6986,7 @@
         <v>37</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L15" s="1">
         <v>2018</v>
@@ -6995,10 +6995,10 @@
         <v>5</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>91</v>
@@ -7010,7 +7010,7 @@
         <v>15044466025</v>
       </c>
       <c r="S15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T15" s="1" t="s">
         <v>77</v>
@@ -7031,30 +7031,30 @@
         <v>77</v>
       </c>
       <c r="AB15" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF15" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="AC15" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD15" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AE15" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AF15" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>61</v>
@@ -7066,7 +7066,7 @@
         <v>37</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L16" s="1">
         <v>2018</v>
@@ -7075,10 +7075,10 @@
         <v>5</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>94</v>
@@ -7090,7 +7090,7 @@
         <v>15044466025</v>
       </c>
       <c r="S16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>78</v>
@@ -7108,30 +7108,30 @@
         <v>44</v>
       </c>
       <c r="AB16" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF16" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="AC16" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD16" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AE16" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AF16" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>61</v>
@@ -7143,7 +7143,7 @@
         <v>37</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L17" s="1">
         <v>2018</v>
@@ -7152,10 +7152,10 @@
         <v>5</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>97</v>
@@ -7167,7 +7167,7 @@
         <v>15044466025</v>
       </c>
       <c r="S17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T17" s="1" t="s">
         <v>79</v>
@@ -7188,20 +7188,93 @@
         <v>79</v>
       </c>
       <c r="AB17" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AC17" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF17" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="AC17" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD17" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AE17" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AF17" s="1" t="s">
-        <v>221</v>
-      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="M22"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="S23"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="S24"/>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="S25"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="S26"/>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="S27"/>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="S28"/>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="S29"/>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="S30"/>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="S31"/>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="S32"/>
+    </row>
+    <row r="33" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S33"/>
+    </row>
+    <row r="34" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S34"/>
+    </row>
+    <row r="35" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S35"/>
+    </row>
+    <row r="36" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S36"/>
+    </row>
+    <row r="38" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S38"/>
+    </row>
+    <row r="39" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S39"/>
+    </row>
+    <row r="40" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S40"/>
+    </row>
+    <row r="41" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S41"/>
+    </row>
+    <row r="42" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S42"/>
+      <c r="Y42" s="3"/>
+    </row>
+    <row r="43" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S43"/>
+    </row>
+    <row r="44" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S44"/>
+    </row>
+    <row r="45" spans="19:25" x14ac:dyDescent="0.25">
+      <c r="S45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added test for purchasing gift certificates via customer-facing
</commit_message>
<xml_diff>
--- a/data/tickets.xlsx
+++ b/data/tickets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Successful" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="251">
   <si>
     <t>id_testdata</t>
   </si>
@@ -566,9 +566,6 @@
     <t>4:15 PM CT</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -774,9 +771,6 @@
   </si>
   <si>
     <t>15</t>
-  </si>
-  <si>
-    <t>13</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1131,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O21" sqref="O21"/>
+      <selection pane="topRight" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,10 +1302,10 @@
         <v>2018</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>181</v>
@@ -1391,7 +1385,7 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>181</v>
@@ -1471,7 +1465,7 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>181</v>
@@ -1551,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>181</v>
@@ -1628,7 +1622,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>181</v>
@@ -1708,7 +1702,7 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>181</v>
@@ -1788,7 +1782,7 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>181</v>
@@ -1868,7 +1862,7 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>181</v>
@@ -1948,7 +1942,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>181</v>
@@ -2028,7 +2022,7 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>181</v>
@@ -2105,7 +2099,7 @@
         <v>5</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>181</v>
@@ -2182,7 +2176,7 @@
         <v>5</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>181</v>
@@ -2262,7 +2256,7 @@
         <v>5</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>181</v>
@@ -2339,7 +2333,7 @@
         <v>5</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>181</v>
@@ -2419,7 +2413,7 @@
         <v>5</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>181</v>
@@ -2496,7 +2490,7 @@
         <v>5</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>181</v>
@@ -2560,9 +2554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,7 +2735,7 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>182</v>
+        <v>250</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>181</v>
@@ -2824,7 +2818,7 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>182</v>
+        <v>250</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>181</v>
@@ -2907,7 +2901,7 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>182</v>
+        <v>250</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>181</v>
@@ -2990,7 +2984,7 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>182</v>
+        <v>250</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>181</v>
@@ -3073,7 +3067,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>182</v>
+        <v>250</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>181</v>
@@ -3156,7 +3150,7 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>182</v>
+        <v>250</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>181</v>
@@ -3239,7 +3233,7 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>182</v>
+        <v>250</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>181</v>
@@ -3322,7 +3316,7 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>182</v>
+        <v>250</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>181</v>
@@ -3405,7 +3399,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>182</v>
+        <v>250</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>181</v>
@@ -3488,7 +3482,7 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>182</v>
+        <v>250</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>181</v>
@@ -3681,19 +3675,19 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F2" s="1">
         <v>2018</v>
@@ -3702,10 +3696,10 @@
         <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>100</v>
@@ -3717,7 +3711,7 @@
         <v>15044466025</v>
       </c>
       <c r="M2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>80</v>
@@ -3738,36 +3732,36 @@
         <v>80</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F3" s="1">
         <v>2018</v>
@@ -3776,10 +3770,10 @@
         <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>113</v>
@@ -3791,7 +3785,7 @@
         <v>15044466025</v>
       </c>
       <c r="M3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>80</v>
@@ -3812,36 +3806,36 @@
         <v>80</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F4" s="1">
         <v>2018</v>
@@ -3850,10 +3844,10 @@
         <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>107</v>
@@ -3865,7 +3859,7 @@
         <v>15044466025</v>
       </c>
       <c r="M4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>81</v>
@@ -3886,36 +3880,36 @@
         <v>35801</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F5" s="1">
         <v>2018</v>
@@ -3924,10 +3918,10 @@
         <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>111</v>
@@ -3939,7 +3933,7 @@
         <v>15044466025</v>
       </c>
       <c r="M5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>81</v>
@@ -3960,36 +3954,36 @@
         <v>35801</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F6" s="1">
         <v>2018</v>
@@ -3998,10 +3992,10 @@
         <v>5</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>117</v>
@@ -4013,7 +4007,7 @@
         <v>15044466025</v>
       </c>
       <c r="M6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>82</v>
@@ -4031,36 +4025,36 @@
         <v>44</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F7" s="1">
         <v>2018</v>
@@ -4069,10 +4063,10 @@
         <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>121</v>
@@ -4084,7 +4078,7 @@
         <v>15044466025</v>
       </c>
       <c r="M7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>82</v>
@@ -4102,36 +4096,36 @@
         <v>44</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F8" s="1">
         <v>2018</v>
@@ -4140,10 +4134,10 @@
         <v>5</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>125</v>
@@ -4155,7 +4149,7 @@
         <v>15044466025</v>
       </c>
       <c r="M8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>83</v>
@@ -4176,36 +4170,36 @@
         <v>83</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F9" s="1">
         <v>2018</v>
@@ -4214,10 +4208,10 @@
         <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>133</v>
@@ -4229,7 +4223,7 @@
         <v>15044466025</v>
       </c>
       <c r="M9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>85</v>
@@ -4247,36 +4241,36 @@
         <v>44</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F10" s="1">
         <v>2018</v>
@@ -4285,10 +4279,10 @@
         <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>127</v>
@@ -4300,7 +4294,7 @@
         <v>15044466025</v>
       </c>
       <c r="M10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>84</v>
@@ -4321,36 +4315,36 @@
         <v>136</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F11" s="1">
         <v>2018</v>
@@ -4359,10 +4353,10 @@
         <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>137</v>
@@ -4374,7 +4368,7 @@
         <v>15044466025</v>
       </c>
       <c r="M11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>85</v>
@@ -4392,36 +4386,36 @@
         <v>44</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F12" s="1">
         <v>2018</v>
@@ -4430,10 +4424,10 @@
         <v>5</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>140</v>
@@ -4445,7 +4439,7 @@
         <v>15044466025</v>
       </c>
       <c r="M12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>86</v>
@@ -4466,48 +4460,48 @@
         <v>143</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F13" s="1">
         <v>2018</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>63</v>
@@ -4519,7 +4513,7 @@
         <v>15044466025</v>
       </c>
       <c r="M13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N13" s="1">
         <v>35801</v>
@@ -4540,36 +4534,36 @@
         <v>35801</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F14" s="1">
         <v>2018</v>
@@ -4578,10 +4572,10 @@
         <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>38</v>
@@ -4593,7 +4587,7 @@
         <v>15044466025</v>
       </c>
       <c r="M14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>76</v>
@@ -4614,36 +4608,36 @@
         <v>76</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F15" s="1">
         <v>2018</v>
@@ -4652,10 +4646,10 @@
         <v>5</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>91</v>
@@ -4667,7 +4661,7 @@
         <v>15044466025</v>
       </c>
       <c r="M15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>77</v>
@@ -4688,36 +4682,36 @@
         <v>77</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F16" s="1">
         <v>2018</v>
@@ -4726,10 +4720,10 @@
         <v>5</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>94</v>
@@ -4741,7 +4735,7 @@
         <v>15044466025</v>
       </c>
       <c r="M16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>78</v>
@@ -4759,36 +4753,36 @@
         <v>44</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F17" s="1">
         <v>2018</v>
@@ -4797,10 +4791,10 @@
         <v>5</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>97</v>
@@ -4812,7 +4806,7 @@
         <v>15044466025</v>
       </c>
       <c r="M17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>79</v>
@@ -4833,19 +4827,19 @@
         <v>79</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -5004,19 +4998,19 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L2" s="1">
         <v>2018</v>
@@ -5025,10 +5019,10 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>63</v>
@@ -5064,36 +5058,36 @@
         <v>35801</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L3" s="1">
         <v>2018</v>
@@ -5102,10 +5096,10 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>38</v>
@@ -5141,36 +5135,36 @@
         <v>76</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L4" s="1">
         <v>2018</v>
@@ -5179,10 +5173,10 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>91</v>
@@ -5218,36 +5212,36 @@
         <v>77</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L5" s="1">
         <v>2018</v>
@@ -5256,10 +5250,10 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>94</v>
@@ -5295,36 +5289,36 @@
         <v>78</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L6" s="1">
         <v>2018</v>
@@ -5333,10 +5327,10 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>97</v>
@@ -5372,36 +5366,36 @@
         <v>79</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L7" s="1">
         <v>2018</v>
@@ -5410,10 +5404,10 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>100</v>
@@ -5434,7 +5428,7 @@
         <v>41</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>157</v>
@@ -5449,36 +5443,36 @@
         <v>80</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF7" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L8" s="1">
         <v>2018</v>
@@ -5487,10 +5481,10 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>113</v>
@@ -5526,36 +5520,36 @@
         <v>80</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF8" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L9" s="1">
         <v>2018</v>
@@ -5564,10 +5558,10 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>107</v>
@@ -5603,36 +5597,36 @@
         <v>80</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE9" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF9" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG9" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L10" s="1">
         <v>2018</v>
@@ -5641,10 +5635,10 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>111</v>
@@ -5680,36 +5674,36 @@
         <v>35801</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG10" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L11" s="1">
         <v>2018</v>
@@ -5718,10 +5712,10 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>117</v>
@@ -5757,19 +5751,19 @@
         <v>76</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF11" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
@@ -5800,7 +5794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C32" sqref="C32"/>
     </sheetView>
@@ -5940,13 +5934,13 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>61</v>
@@ -5958,7 +5952,7 @@
         <v>37</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L2" s="1">
         <v>2018</v>
@@ -5967,10 +5961,10 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>100</v>
@@ -5982,7 +5976,7 @@
         <v>15044466025</v>
       </c>
       <c r="S2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>80</v>
@@ -6003,30 +5997,30 @@
         <v>80</v>
       </c>
       <c r="AB2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="AC2" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="AF2" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>61</v>
@@ -6038,7 +6032,7 @@
         <v>37</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L3" s="1">
         <v>2018</v>
@@ -6047,10 +6041,10 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>113</v>
@@ -6062,7 +6056,7 @@
         <v>15044466025</v>
       </c>
       <c r="S3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>80</v>
@@ -6083,30 +6077,30 @@
         <v>80</v>
       </c>
       <c r="AB3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="AC3" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AE3" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="AF3" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>61</v>
@@ -6118,7 +6112,7 @@
         <v>37</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L4" s="1">
         <v>2018</v>
@@ -6127,10 +6121,10 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>107</v>
@@ -6142,7 +6136,7 @@
         <v>15044466025</v>
       </c>
       <c r="S4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>81</v>
@@ -6163,30 +6157,30 @@
         <v>35801</v>
       </c>
       <c r="AB4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD4" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="AC4" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AE4" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="AF4" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>61</v>
@@ -6198,7 +6192,7 @@
         <v>37</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L5" s="1">
         <v>2018</v>
@@ -6207,10 +6201,10 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>111</v>
@@ -6222,7 +6216,7 @@
         <v>15044466025</v>
       </c>
       <c r="S5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>81</v>
@@ -6243,30 +6237,30 @@
         <v>35801</v>
       </c>
       <c r="AB5" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD5" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="AC5" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AE5" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="AF5" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>61</v>
@@ -6278,7 +6272,7 @@
         <v>37</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L6" s="1">
         <v>2018</v>
@@ -6287,10 +6281,10 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>117</v>
@@ -6302,7 +6296,7 @@
         <v>15044466025</v>
       </c>
       <c r="S6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>82</v>
@@ -6320,30 +6314,30 @@
         <v>44</v>
       </c>
       <c r="AB6" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD6" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="AC6" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AE6" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AE6" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="AF6" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>61</v>
@@ -6355,7 +6349,7 @@
         <v>37</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L7" s="1">
         <v>2018</v>
@@ -6364,10 +6358,10 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>121</v>
@@ -6379,7 +6373,7 @@
         <v>15044466025</v>
       </c>
       <c r="S7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>82</v>
@@ -6397,30 +6391,30 @@
         <v>44</v>
       </c>
       <c r="AB7" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF7" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="AE7" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AF7" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>61</v>
@@ -6432,7 +6426,7 @@
         <v>37</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L8" s="1">
         <v>2018</v>
@@ -6441,10 +6435,10 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>125</v>
@@ -6456,7 +6450,7 @@
         <v>15044466025</v>
       </c>
       <c r="S8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>83</v>
@@ -6477,30 +6471,30 @@
         <v>83</v>
       </c>
       <c r="AB8" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF8" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="AE8" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AF8" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>61</v>
@@ -6512,7 +6506,7 @@
         <v>37</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L9" s="1">
         <v>2018</v>
@@ -6521,10 +6515,10 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>133</v>
@@ -6536,7 +6530,7 @@
         <v>15044466025</v>
       </c>
       <c r="S9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>85</v>
@@ -6554,30 +6548,30 @@
         <v>44</v>
       </c>
       <c r="AB9" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF9" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD9" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="AE9" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AF9" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>61</v>
@@ -6589,7 +6583,7 @@
         <v>37</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L10" s="1">
         <v>2018</v>
@@ -6598,10 +6592,10 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>127</v>
@@ -6613,7 +6607,7 @@
         <v>15044466025</v>
       </c>
       <c r="S10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>84</v>
@@ -6634,30 +6628,30 @@
         <v>136</v>
       </c>
       <c r="AB10" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF10" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="AC10" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD10" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="AE10" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AF10" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>61</v>
@@ -6669,7 +6663,7 @@
         <v>37</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L11" s="1">
         <v>2018</v>
@@ -6678,10 +6672,10 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>137</v>
@@ -6693,7 +6687,7 @@
         <v>15044466025</v>
       </c>
       <c r="S11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>85</v>
@@ -6711,30 +6705,30 @@
         <v>44</v>
       </c>
       <c r="AB11" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF11" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD11" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="AE11" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AF11" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>61</v>
@@ -6746,7 +6740,7 @@
         <v>37</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L12" s="1">
         <v>2018</v>
@@ -6755,10 +6749,10 @@
         <v>5</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>140</v>
@@ -6770,7 +6764,7 @@
         <v>15044466025</v>
       </c>
       <c r="S12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>86</v>
@@ -6791,30 +6785,30 @@
         <v>143</v>
       </c>
       <c r="AB12" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF12" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="AE12" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AF12" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -6826,19 +6820,19 @@
         <v>37</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L13" s="1">
         <v>2018</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>63</v>
@@ -6850,7 +6844,7 @@
         <v>15044466025</v>
       </c>
       <c r="S13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T13" s="1">
         <v>35801</v>
@@ -6871,30 +6865,30 @@
         <v>35801</v>
       </c>
       <c r="AB13" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF13" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="AE13" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AF13" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -6906,7 +6900,7 @@
         <v>37</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L14" s="1">
         <v>2018</v>
@@ -6915,10 +6909,10 @@
         <v>5</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>38</v>
@@ -6930,7 +6924,7 @@
         <v>15044466025</v>
       </c>
       <c r="S14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="T14" s="1" t="s">
         <v>76</v>
@@ -6951,30 +6945,30 @@
         <v>76</v>
       </c>
       <c r="AB14" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF14" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD14" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="AE14" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AF14" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -6986,7 +6980,7 @@
         <v>37</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L15" s="1">
         <v>2018</v>
@@ -6995,10 +6989,10 @@
         <v>5</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>91</v>
@@ -7010,7 +7004,7 @@
         <v>15044466025</v>
       </c>
       <c r="S15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T15" s="1" t="s">
         <v>77</v>
@@ -7031,30 +7025,30 @@
         <v>77</v>
       </c>
       <c r="AB15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF15" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="AC15" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD15" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="AE15" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AF15" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>61</v>
@@ -7066,7 +7060,7 @@
         <v>37</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L16" s="1">
         <v>2018</v>
@@ -7075,10 +7069,10 @@
         <v>5</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>94</v>
@@ -7090,7 +7084,7 @@
         <v>15044466025</v>
       </c>
       <c r="S16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>78</v>
@@ -7108,30 +7102,30 @@
         <v>44</v>
       </c>
       <c r="AB16" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF16" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="AC16" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD16" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="AE16" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AF16" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>61</v>
@@ -7143,7 +7137,7 @@
         <v>37</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L17" s="1">
         <v>2018</v>
@@ -7152,10 +7146,10 @@
         <v>5</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>97</v>
@@ -7167,7 +7161,7 @@
         <v>15044466025</v>
       </c>
       <c r="S17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T17" s="1" t="s">
         <v>79</v>
@@ -7188,19 +7182,19 @@
         <v>79</v>
       </c>
       <c r="AB17" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF17" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="AC17" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD17" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="AE17" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AF17" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added test data for booking with cash.
</commit_message>
<xml_diff>
--- a/data/tickets.xlsx
+++ b/data/tickets.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Successful" sheetId="1" r:id="rId1"/>
     <sheet name="Declined" sheetId="2" r:id="rId2"/>
     <sheet name="Customer Successful" sheetId="4" r:id="rId3"/>
     <sheet name="Customer Declined" sheetId="5" r:id="rId4"/>
-    <sheet name="Customer Successful--" sheetId="3" r:id="rId5"/>
+    <sheet name="Customer Successful--AlertTest" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="333">
   <si>
     <t>id_testdata</t>
   </si>
@@ -770,7 +770,253 @@
     <t>GoDo-710</t>
   </si>
   <si>
-    <t>15</t>
+    <t>GHO0001_NNCU1SC</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Judy</t>
+  </si>
+  <si>
+    <t>Viola</t>
+  </si>
+  <si>
+    <t>Chandler</t>
+  </si>
+  <si>
+    <t>Ernest</t>
+  </si>
+  <si>
+    <t>Webb</t>
+  </si>
+  <si>
+    <t>Cedric</t>
+  </si>
+  <si>
+    <t>Singleton</t>
+  </si>
+  <si>
+    <t>Christy</t>
+  </si>
+  <si>
+    <t>Vargas</t>
+  </si>
+  <si>
+    <t>Rosalie</t>
+  </si>
+  <si>
+    <t>Benson</t>
+  </si>
+  <si>
+    <t>Jackie</t>
+  </si>
+  <si>
+    <t>Becker</t>
+  </si>
+  <si>
+    <t>Harriet</t>
+  </si>
+  <si>
+    <t>Glover</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Wise</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Vaughn</t>
+  </si>
+  <si>
+    <t>Amette-Spock</t>
+  </si>
+  <si>
+    <t>Saul</t>
+  </si>
+  <si>
+    <t>Rodriquez</t>
+  </si>
+  <si>
+    <t>Harold</t>
+  </si>
+  <si>
+    <t>Rios</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>Lewis</t>
+  </si>
+  <si>
+    <t>Emanuel</t>
+  </si>
+  <si>
+    <t>Dawson</t>
+  </si>
+  <si>
+    <t>Gilbert</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Allen</t>
+  </si>
+  <si>
+    <t>Emilio</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Geoffrey</t>
+  </si>
+  <si>
+    <t>Graham</t>
+  </si>
+  <si>
+    <t>Jasmine</t>
+  </si>
+  <si>
+    <t>Wells</t>
+  </si>
+  <si>
+    <t>Neal</t>
+  </si>
+  <si>
+    <t>Hayes</t>
+  </si>
+  <si>
+    <t>Brad</t>
+  </si>
+  <si>
+    <t>Lane</t>
+  </si>
+  <si>
+    <t>Lorene</t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>Gladys</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>Gail</t>
+  </si>
+  <si>
+    <t>O'brien</t>
+  </si>
+  <si>
+    <t>Bert</t>
+  </si>
+  <si>
+    <t>Horton</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Perkins</t>
+  </si>
+  <si>
+    <t>Bradford</t>
+  </si>
+  <si>
+    <t>Cruz</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>Hunt</t>
+  </si>
+  <si>
+    <t>Dana</t>
+  </si>
+  <si>
+    <t>Munoz</t>
+  </si>
+  <si>
+    <t>Courtney</t>
+  </si>
+  <si>
+    <t>Jefferson</t>
+  </si>
+  <si>
+    <t>Christie</t>
+  </si>
+  <si>
+    <t>Tran</t>
+  </si>
+  <si>
+    <t>Carlton</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Elaine</t>
+  </si>
+  <si>
+    <t>Phelps</t>
+  </si>
+  <si>
+    <t>Bryan</t>
+  </si>
+  <si>
+    <t>Riley</t>
+  </si>
+  <si>
+    <t>GoDo-Cash +</t>
+  </si>
+  <si>
+    <t>GoDo-Cash -</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Maxey</t>
+  </si>
+  <si>
+    <t>Vallie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marlin </t>
+  </si>
+  <si>
+    <t>Hutchison</t>
+  </si>
+  <si>
+    <t>godo-cash+@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-cash-@mailinator.com</t>
+  </si>
+  <si>
+    <t>28</t>
   </si>
 </sst>
 </file>
@@ -1127,11 +1373,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI17"/>
+  <dimension ref="A1:AI19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,7 +1527,7 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>322</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>180</v>
@@ -1305,40 +1551,31 @@
         <v>182</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>250</v>
+        <v>332</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>63</v>
+        <v>327</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>64</v>
+        <v>326</v>
       </c>
       <c r="R2" s="1">
         <v>15044466025</v>
       </c>
       <c r="S2" t="s">
-        <v>65</v>
+        <v>330</v>
       </c>
       <c r="T2" s="1">
         <v>35801</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>35801</v>
+        <v>325</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>45</v>
@@ -1361,7 +1598,7 @@
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>323</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>180</v>
@@ -1381,44 +1618,32 @@
       <c r="L3" s="1">
         <v>2018</v>
       </c>
-      <c r="M3" s="1">
-        <v>5</v>
+      <c r="M3" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>250</v>
+        <v>332</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>38</v>
+        <v>328</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>39</v>
+        <v>329</v>
       </c>
       <c r="R3" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>76</v>
+      <c r="S3" t="s">
+        <v>331</v>
+      </c>
+      <c r="T3" s="1">
+        <v>35801</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>76</v>
+        <v>325</v>
       </c>
       <c r="AD3" s="1" t="s">
         <v>45</v>
@@ -1441,7 +1666,7 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>180</v>
@@ -1461,35 +1686,35 @@
       <c r="L4" s="1">
         <v>2018</v>
       </c>
-      <c r="M4" s="1">
-        <v>5</v>
+      <c r="M4" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="R4" s="1">
         <v>15044466025</v>
       </c>
       <c r="S4" t="s">
-        <v>66</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
+      </c>
+      <c r="T4" s="1">
+        <v>35801</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Z4" s="1" t="s">
         <v>43</v>
@@ -1497,8 +1722,8 @@
       <c r="AA4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AB4" s="1" t="s">
-        <v>77</v>
+      <c r="AB4" s="1">
+        <v>35801</v>
       </c>
       <c r="AD4" s="1" t="s">
         <v>45</v>
@@ -1521,7 +1746,7 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>180</v>
@@ -1529,8 +1754,8 @@
       <c r="C5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>61</v>
+      <c r="D5" s="1">
+        <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>36</v>
@@ -1545,31 +1770,31 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="R5" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S5" t="s">
-        <v>67</v>
+      <c r="S5" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="Z5" s="1" t="s">
         <v>43</v>
@@ -1577,6 +1802,9 @@
       <c r="AA5" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="AB5" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="AD5" s="1" t="s">
         <v>45</v>
       </c>
@@ -1598,7 +1826,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>180</v>
@@ -1606,8 +1834,8 @@
       <c r="C6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>61</v>
+      <c r="D6" s="1">
+        <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>36</v>
@@ -1622,31 +1850,31 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="R6" s="1">
         <v>15044466025</v>
       </c>
       <c r="S6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z6" s="1" t="s">
         <v>43</v>
@@ -1655,7 +1883,7 @@
         <v>44</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AD6" s="1" t="s">
         <v>45</v>
@@ -1678,7 +1906,7 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>180</v>
@@ -1702,40 +1930,37 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="R7" s="1">
         <v>15044466025</v>
       </c>
       <c r="S7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Z7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="AD7" s="1" t="s">
         <v>45</v>
@@ -1758,7 +1983,7 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>180</v>
@@ -1782,40 +2007,40 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="R8" s="1">
         <v>15044466025</v>
       </c>
       <c r="S8" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W8" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="Z8" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AD8" s="1" t="s">
         <v>45</v>
@@ -1838,7 +2063,7 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>180</v>
@@ -1862,40 +2087,40 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="R9" s="1">
         <v>15044466025</v>
       </c>
       <c r="S9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="Z9" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB9" s="1">
-        <v>35801</v>
+        <v>103</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="AD9" s="1" t="s">
         <v>45</v>
@@ -1918,7 +2143,7 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>180</v>
@@ -1942,40 +2167,40 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="R10" s="1">
         <v>15044466025</v>
       </c>
       <c r="S10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="Z10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB10" s="1">
-        <v>35801</v>
+        <v>103</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="AD10" s="1" t="s">
         <v>45</v>
@@ -1998,7 +2223,7 @@
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>180</v>
@@ -2006,7 +2231,7 @@
       <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -2022,31 +2247,31 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="R11" s="1">
         <v>15044466025</v>
       </c>
       <c r="S11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="Z11" s="1" t="s">
         <v>43</v>
@@ -2054,8 +2279,11 @@
       <c r="AA11" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="AB11" s="1">
+        <v>35801</v>
+      </c>
       <c r="AD11" s="1" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="AE11" s="1" t="s">
         <v>46</v>
@@ -2064,18 +2292,18 @@
         <v>46</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="AH11" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>180</v>
@@ -2083,7 +2311,7 @@
       <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -2099,31 +2327,31 @@
         <v>5</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="R12" s="1">
         <v>15044466025</v>
       </c>
       <c r="S12" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="W12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="Z12" s="1" t="s">
         <v>43</v>
@@ -2131,8 +2359,11 @@
       <c r="AA12" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="AB12" s="1">
+        <v>35801</v>
+      </c>
       <c r="AD12" s="1" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="AE12" s="1" t="s">
         <v>46</v>
@@ -2141,18 +2372,18 @@
         <v>46</v>
       </c>
       <c r="AG12" s="1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="AH12" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>180</v>
@@ -2176,31 +2407,31 @@
         <v>5</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="R13" s="1">
         <v>15044466025</v>
       </c>
       <c r="S13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="W13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="Z13" s="1" t="s">
         <v>43</v>
@@ -2208,9 +2439,6 @@
       <c r="AA13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AB13" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="AD13" s="1" t="s">
         <v>89</v>
       </c>
@@ -2232,7 +2460,7 @@
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>180</v>
@@ -2256,31 +2484,31 @@
         <v>5</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="R14" s="1">
         <v>15044466025</v>
       </c>
       <c r="S14" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="W14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="Z14" s="1" t="s">
         <v>43</v>
@@ -2309,7 +2537,7 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>180</v>
@@ -2333,31 +2561,31 @@
         <v>5</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="R15" s="1">
         <v>15044466025</v>
       </c>
       <c r="S15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="W15" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="Z15" s="1" t="s">
         <v>43</v>
@@ -2366,7 +2594,7 @@
         <v>44</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>136</v>
+        <v>83</v>
       </c>
       <c r="AD15" s="1" t="s">
         <v>89</v>
@@ -2389,7 +2617,7 @@
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>180</v>
@@ -2413,22 +2641,22 @@
         <v>5</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="R16" s="1">
         <v>15044466025</v>
       </c>
       <c r="S16" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>85</v>
@@ -2437,7 +2665,7 @@
         <v>41</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="Z16" s="1" t="s">
         <v>43</v>
@@ -2466,7 +2694,7 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>180</v>
@@ -2490,31 +2718,31 @@
         <v>5</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="R17" s="1">
         <v>15044466025</v>
       </c>
       <c r="S17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="W17" s="1" t="s">
         <v>41</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="Z17" s="1" t="s">
         <v>43</v>
@@ -2523,7 +2751,7 @@
         <v>44</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="AD17" s="1" t="s">
         <v>89</v>
@@ -2541,6 +2769,163 @@
         <v>49</v>
       </c>
       <c r="AI17" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M18" s="1">
+        <v>5</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="R18" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S18" t="s">
+        <v>74</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI18" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M19" s="1">
+        <v>5</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="R19" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="S19" t="s">
+        <v>75</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI19" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2554,9 +2939,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N16" sqref="N16"/>
+      <selection pane="topRight" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2574,7 +2959,7 @@
     <col min="11" max="11" width="25.28515625" style="1" customWidth="1"/>
     <col min="12" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="13.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" style="1" customWidth="1"/>
     <col min="17" max="17" width="14.42578125" style="1" customWidth="1"/>
     <col min="18" max="18" width="20.28515625" style="1" customWidth="1"/>
     <col min="19" max="19" width="38.28515625" style="1" customWidth="1"/>
@@ -2735,16 +3120,16 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>63</v>
+        <v>254</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="R2" s="1">
         <v>15044466025</v>
@@ -2818,16 +3203,16 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>38</v>
+        <v>255</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>39</v>
+        <v>256</v>
       </c>
       <c r="R3" s="1">
         <v>15044466025</v>
@@ -2901,16 +3286,16 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>91</v>
+        <v>257</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>92</v>
+        <v>258</v>
       </c>
       <c r="R4" s="1">
         <v>15044466025</v>
@@ -2984,16 +3369,16 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>94</v>
+        <v>259</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>95</v>
+        <v>260</v>
       </c>
       <c r="R5" s="1">
         <v>15044466025</v>
@@ -3067,16 +3452,16 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>98</v>
+        <v>262</v>
       </c>
       <c r="R6" s="1">
         <v>15044466025</v>
@@ -3150,16 +3535,16 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>100</v>
+        <v>263</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>101</v>
+        <v>264</v>
       </c>
       <c r="R7" s="1">
         <v>15044466025</v>
@@ -3233,16 +3618,16 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>113</v>
+        <v>265</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>114</v>
+        <v>266</v>
       </c>
       <c r="R8" s="1">
         <v>15044466025</v>
@@ -3316,16 +3701,16 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>107</v>
+        <v>267</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>108</v>
+        <v>268</v>
       </c>
       <c r="R9" s="1">
         <v>15044466025</v>
@@ -3399,16 +3784,16 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>111</v>
+        <v>269</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>112</v>
+        <v>270</v>
       </c>
       <c r="R10" s="1">
         <v>15044466025</v>
@@ -3482,16 +3867,16 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>117</v>
+        <v>271</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>118</v>
+        <v>272</v>
       </c>
       <c r="R11" s="1">
         <v>15044466025</v>
@@ -3567,9 +3952,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B23" sqref="B23"/>
+      <selection pane="topRight" activeCell="H23" sqref="A23:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3696,7 +4081,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>236</v>
@@ -3705,7 +4090,7 @@
         <v>100</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>101</v>
+        <v>273</v>
       </c>
       <c r="L2" s="1">
         <v>15044466025</v>
@@ -3770,16 +4155,16 @@
         <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>113</v>
+        <v>274</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>114</v>
+        <v>275</v>
       </c>
       <c r="L3" s="1">
         <v>15044466025</v>
@@ -3844,16 +4229,16 @@
         <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>107</v>
+        <v>276</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>108</v>
+        <v>277</v>
       </c>
       <c r="L4" s="1">
         <v>15044466025</v>
@@ -3918,16 +4303,16 @@
         <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>111</v>
+        <v>278</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>112</v>
+        <v>279</v>
       </c>
       <c r="L5" s="1">
         <v>15044466025</v>
@@ -3992,16 +4377,16 @@
         <v>5</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>117</v>
+        <v>280</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>118</v>
+        <v>281</v>
       </c>
       <c r="L6" s="1">
         <v>15044466025</v>
@@ -4063,16 +4448,16 @@
         <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>121</v>
+        <v>282</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>122</v>
+        <v>283</v>
       </c>
       <c r="L7" s="1">
         <v>15044466025</v>
@@ -4134,16 +4519,16 @@
         <v>5</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>125</v>
+        <v>284</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>126</v>
+        <v>285</v>
       </c>
       <c r="L8" s="1">
         <v>15044466025</v>
@@ -4208,7 +4593,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>236</v>
@@ -4279,16 +4664,16 @@
         <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>127</v>
+        <v>286</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>128</v>
+        <v>287</v>
       </c>
       <c r="L10" s="1">
         <v>15044466025</v>
@@ -4353,16 +4738,16 @@
         <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>137</v>
+        <v>288</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>138</v>
+        <v>289</v>
       </c>
       <c r="L11" s="1">
         <v>15044466025</v>
@@ -4424,16 +4809,16 @@
         <v>5</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>140</v>
+        <v>290</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>141</v>
+        <v>291</v>
       </c>
       <c r="L12" s="1">
         <v>15044466025</v>
@@ -4498,16 +4883,16 @@
         <v>182</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>63</v>
+        <v>292</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>64</v>
+        <v>293</v>
       </c>
       <c r="L13" s="1">
         <v>15044466025</v>
@@ -4572,16 +4957,16 @@
         <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>38</v>
+        <v>294</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>39</v>
+        <v>295</v>
       </c>
       <c r="L14" s="1">
         <v>15044466025</v>
@@ -4646,16 +5031,16 @@
         <v>5</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>91</v>
+        <v>296</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>92</v>
+        <v>297</v>
       </c>
       <c r="L15" s="1">
         <v>15044466025</v>
@@ -4720,16 +5105,16 @@
         <v>5</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>94</v>
+        <v>298</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>95</v>
+        <v>299</v>
       </c>
       <c r="L16" s="1">
         <v>15044466025</v>
@@ -4791,16 +5176,16 @@
         <v>5</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>236</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>97</v>
+        <v>300</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>98</v>
+        <v>301</v>
       </c>
       <c r="L17" s="1">
         <v>15044466025</v>
@@ -4853,8 +5238,8 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N16" sqref="N16"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5019,16 +5404,16 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>63</v>
+        <v>302</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>64</v>
+        <v>303</v>
       </c>
       <c r="R2" s="1">
         <v>15044466025</v>
@@ -5038,6 +5423,9 @@
       </c>
       <c r="T2" s="1">
         <v>35801</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>41</v>
@@ -5096,16 +5484,16 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>38</v>
+        <v>304</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>39</v>
+        <v>305</v>
       </c>
       <c r="R3" s="1">
         <v>15044466025</v>
@@ -5115,6 +5503,9 @@
       </c>
       <c r="T3" s="1" t="s">
         <v>76</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>41</v>
@@ -5173,16 +5564,16 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>91</v>
+        <v>306</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>92</v>
+        <v>307</v>
       </c>
       <c r="R4" s="1">
         <v>15044466025</v>
@@ -5192,6 +5583,9 @@
       </c>
       <c r="T4" s="1" t="s">
         <v>77</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>41</v>
@@ -5250,16 +5644,16 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>94</v>
+        <v>308</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>95</v>
+        <v>309</v>
       </c>
       <c r="R5" s="1">
         <v>15044466025</v>
@@ -5269,6 +5663,9 @@
       </c>
       <c r="T5" s="1" t="s">
         <v>78</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>41</v>
@@ -5327,16 +5724,16 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>97</v>
+        <v>310</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>98</v>
+        <v>311</v>
       </c>
       <c r="R6" s="1">
         <v>15044466025</v>
@@ -5346,6 +5743,9 @@
       </c>
       <c r="T6" s="1" t="s">
         <v>79</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>41</v>
@@ -5404,16 +5804,16 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>100</v>
+        <v>312</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>101</v>
+        <v>313</v>
       </c>
       <c r="R7" s="1">
         <v>15044466025</v>
@@ -5423,6 +5823,9 @@
       </c>
       <c r="T7" s="1" t="s">
         <v>80</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>41</v>
@@ -5481,16 +5884,16 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>113</v>
+        <v>314</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>114</v>
+        <v>315</v>
       </c>
       <c r="R8" s="1">
         <v>15044466025</v>
@@ -5500,6 +5903,9 @@
       </c>
       <c r="T8" s="1" t="s">
         <v>80</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="W8" s="1" t="s">
         <v>41</v>
@@ -5558,16 +5964,16 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>107</v>
+        <v>316</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>108</v>
+        <v>317</v>
       </c>
       <c r="R9" s="1">
         <v>15044466025</v>
@@ -5577,6 +5983,9 @@
       </c>
       <c r="T9" s="1" t="s">
         <v>81</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>41</v>
@@ -5635,16 +6044,16 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>111</v>
+        <v>318</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>112</v>
+        <v>319</v>
       </c>
       <c r="R10" s="1">
         <v>15044466025</v>
@@ -5654,6 +6063,9 @@
       </c>
       <c r="T10" s="1" t="s">
         <v>81</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>41</v>
@@ -5712,16 +6124,16 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>117</v>
+        <v>320</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>118</v>
+        <v>321</v>
       </c>
       <c r="R11" s="1">
         <v>15044466025</v>
@@ -5731,6 +6143,9 @@
       </c>
       <c r="T11" s="1" t="s">
         <v>82</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>41</v>
@@ -5796,7 +6211,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C32" sqref="C32"/>
+      <selection pane="topRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added test for successfully applying promo codes.
</commit_message>
<xml_diff>
--- a/data/tickets.xlsx
+++ b/data/tickets.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="419">
   <si>
     <t>id_testdata</t>
   </si>
@@ -1016,7 +1016,265 @@
     <t>godo-cash-@mailinator.com</t>
   </si>
   <si>
-    <t>28</t>
+    <t>23</t>
+  </si>
+  <si>
+    <t>2:00 PM CT</t>
+  </si>
+  <si>
+    <t>GoDo-279</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>278REGRESS</t>
+  </si>
+  <si>
+    <t>godo-279@mailinator.com</t>
+  </si>
+  <si>
+    <t>Megan</t>
+  </si>
+  <si>
+    <t>Fitzgerald</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>11:30 AM CT</t>
+  </si>
+  <si>
+    <t>$200.00</t>
+  </si>
+  <si>
+    <t>$18.50</t>
+  </si>
+  <si>
+    <t>$203.50</t>
+  </si>
+  <si>
+    <t>- $15.00</t>
+  </si>
+  <si>
+    <t>GoDo-280</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Kelli</t>
+  </si>
+  <si>
+    <t>Owen</t>
+  </si>
+  <si>
+    <t>godo-280@mailinator.com</t>
+  </si>
+  <si>
+    <t>29130</t>
+  </si>
+  <si>
+    <t>$300.00</t>
+  </si>
+  <si>
+    <t>$28.50</t>
+  </si>
+  <si>
+    <t>$313.50</t>
+  </si>
+  <si>
+    <t>GoDo-292</t>
+  </si>
+  <si>
+    <t>Climbing</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Dewey</t>
+  </si>
+  <si>
+    <t>Jensen</t>
+  </si>
+  <si>
+    <t>godo-292@mailinator.com</t>
+  </si>
+  <si>
+    <t>89611</t>
+  </si>
+  <si>
+    <t>CASE123</t>
+  </si>
+  <si>
+    <t>2:00 PM AT</t>
+  </si>
+  <si>
+    <t>$45.00</t>
+  </si>
+  <si>
+    <t>- $4.50</t>
+  </si>
+  <si>
+    <t>$4.05</t>
+  </si>
+  <si>
+    <t>$44.55</t>
+  </si>
+  <si>
+    <t>GoDo-293</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Belinda</t>
+  </si>
+  <si>
+    <t>Gonzalez</t>
+  </si>
+  <si>
+    <t>godo-293@mailinator.com</t>
+  </si>
+  <si>
+    <t>71502</t>
+  </si>
+  <si>
+    <t>$50.00</t>
+  </si>
+  <si>
+    <t>- $5.00</t>
+  </si>
+  <si>
+    <t>$4.50</t>
+  </si>
+  <si>
+    <t>$49.50</t>
+  </si>
+  <si>
+    <t>GoDo-297</t>
+  </si>
+  <si>
+    <t>Five dollars</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>11:10 AM CT</t>
+  </si>
+  <si>
+    <t>Jeremy</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>godo-297@mailinator.com</t>
+  </si>
+  <si>
+    <t>60156</t>
+  </si>
+  <si>
+    <t>- $2.00</t>
+  </si>
+  <si>
+    <t>$0.90</t>
+  </si>
+  <si>
+    <t>$18.90</t>
+  </si>
+  <si>
+    <t>GoDo-298</t>
+  </si>
+  <si>
+    <t>ccccc</t>
+  </si>
+  <si>
+    <t>10:00 AM CT</t>
+  </si>
+  <si>
+    <t>adult</t>
+  </si>
+  <si>
+    <t>child</t>
+  </si>
+  <si>
+    <t>$20.01</t>
+  </si>
+  <si>
+    <t>$0.18</t>
+  </si>
+  <si>
+    <t>$18.19</t>
+  </si>
+  <si>
+    <t>59701</t>
+  </si>
+  <si>
+    <t>godo-298@mailinator.com</t>
+  </si>
+  <si>
+    <t>Dwight</t>
+  </si>
+  <si>
+    <t>GoDo-301</t>
+  </si>
+  <si>
+    <t>Ferdinand</t>
+  </si>
+  <si>
+    <t>Bruton</t>
+  </si>
+  <si>
+    <t>godo-301@mailinator.com</t>
+  </si>
+  <si>
+    <t>GoDo-305</t>
+  </si>
+  <si>
+    <t>Germaine</t>
+  </si>
+  <si>
+    <t>Callender</t>
+  </si>
+  <si>
+    <t>godo-305@mailinator.com</t>
+  </si>
+  <si>
+    <t>19380</t>
+  </si>
+  <si>
+    <t>FROMTO</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>GoDo-306</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>Latricia</t>
+  </si>
+  <si>
+    <t>Ouellette</t>
+  </si>
+  <si>
+    <t>godo-306@mailinator.com</t>
+  </si>
+  <si>
+    <t>10:20 AM AT</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1299,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1051,6 +1309,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1067,11 +1337,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1373,1560 +1645,2114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI19"/>
+  <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" style="1" customWidth="1"/>
-    <col min="12" max="14" width="9.140625" style="1"/>
-    <col min="15" max="15" width="13.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="20.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="38.28515625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="12.28515625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="18.85546875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="20.42578125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="15.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="18.5703125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="20" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="12.28515625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11" style="1" customWidth="1"/>
-    <col min="29" max="29" width="14.140625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="13.28515625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="10.5703125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="15" style="1" customWidth="1"/>
-    <col min="33" max="33" width="13.7109375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="15" style="1" customWidth="1"/>
-    <col min="35" max="35" width="15.42578125" style="1" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="27.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="1" customWidth="1"/>
+    <col min="11" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="13.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="38.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="20.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="18.5703125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="20" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.85546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="11" style="1" customWidth="1"/>
+    <col min="28" max="28" width="14.140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="13.28515625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5703125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15" style="1" customWidth="1"/>
+    <col min="32" max="32" width="13.7109375" style="1" customWidth="1"/>
+    <col min="33" max="33" width="15" style="1" customWidth="1"/>
+    <col min="34" max="34" width="15.42578125" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>322</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="1">
+      <c r="K2" s="1">
         <v>2018</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="M2" s="1" t="s">
-        <v>182</v>
+        <v>251</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>181</v>
+        <v>327</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q2" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="R2" s="1">
+      <c r="Q2" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S2" t="s">
+      <c r="R2" t="s">
         <v>330</v>
       </c>
-      <c r="T2" s="1">
+      <c r="S2" s="1">
         <v>35801</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>325</v>
       </c>
+      <c r="AB2" s="1" t="s">
+        <v>324</v>
+      </c>
       <c r="AC2" s="1" t="s">
-        <v>324</v>
+        <v>45</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI2" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>323</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="1">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="1">
+      <c r="K3" s="1">
         <v>2018</v>
       </c>
+      <c r="L3" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="M3" s="1" t="s">
-        <v>182</v>
+        <v>251</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>181</v>
+        <v>328</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="Q3" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="R3" s="1">
+      <c r="Q3" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S3" t="s">
+      <c r="R3" t="s">
         <v>331</v>
       </c>
-      <c r="T3" s="1">
+      <c r="S3" s="1">
         <v>35801</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>325</v>
       </c>
+      <c r="AC3" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="AD3" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE3" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI3" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="1">
+      <c r="C4" s="1">
         <v>1</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="1">
+      <c r="K4" s="1">
         <v>2018</v>
       </c>
+      <c r="L4" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="M4" s="1" t="s">
-        <v>182</v>
+        <v>251</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>181</v>
+        <v>63</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R4" s="1">
+      <c r="Q4" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S4" t="s">
+      <c r="R4" t="s">
         <v>65</v>
       </c>
-      <c r="T4" s="1">
+      <c r="S4" s="1">
         <v>35801</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X4" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="Y4" s="1" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AA4" s="1">
         <v>35801</v>
       </c>
+      <c r="AC4" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="AD4" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE4" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI4" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="1">
+      <c r="C5" s="1">
         <v>1</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K5" s="1">
+        <v>2018</v>
+      </c>
       <c r="L5" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M5" s="1">
         <v>5</v>
       </c>
+      <c r="M5" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N5" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>181</v>
+        <v>38</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R5" s="1">
+      <c r="Q5" s="1">
         <v>15044466025</v>
       </c>
+      <c r="R5" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="S5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X5" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="Y5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB5" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="AC5" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="AD5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE5" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI5" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="1">
+      <c r="C6" s="1">
         <v>1</v>
       </c>
+      <c r="G6" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K6" s="1">
+        <v>2018</v>
+      </c>
       <c r="L6" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M6" s="1">
         <v>5</v>
       </c>
+      <c r="M6" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N6" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>181</v>
+        <v>91</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R6" s="1">
+      <c r="Q6" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S6" t="s">
+      <c r="R6" t="s">
         <v>66</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X6" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="Y6" s="1" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB6" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="AC6" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="AD6" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE6" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI6" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>180</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K7" s="1">
+        <v>2018</v>
+      </c>
       <c r="L7" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M7" s="1">
         <v>5</v>
       </c>
+      <c r="M7" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N7" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>181</v>
+        <v>94</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q7" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="R7" s="1">
+      <c r="Q7" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S7" t="s">
+      <c r="R7" t="s">
         <v>67</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X7" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="Y7" s="1" t="s">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA7" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="AC7" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="AD7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE7" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF7" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI7" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>180</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K8" s="1">
+        <v>2018</v>
+      </c>
       <c r="L8" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M8" s="1">
         <v>5</v>
       </c>
+      <c r="M8" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N8" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>181</v>
+        <v>97</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q8" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="R8" s="1">
+      <c r="Q8" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S8" t="s">
+      <c r="R8" t="s">
         <v>68</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X8" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="Y8" s="1" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB8" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="AC8" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="AD8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF8" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI8" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>180</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K9" s="1">
+        <v>2018</v>
+      </c>
       <c r="L9" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M9" s="1">
         <v>5</v>
       </c>
+      <c r="M9" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N9" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>181</v>
+        <v>100</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q9" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="R9" s="1">
+      <c r="Q9" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S9" t="s">
+      <c r="R9" t="s">
         <v>69</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X9" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="Y9" s="1" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB9" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="AC9" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="AD9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE9" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF9" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI9" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>180</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K10" s="1">
+        <v>2018</v>
+      </c>
       <c r="L10" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M10" s="1">
         <v>5</v>
       </c>
+      <c r="M10" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N10" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>181</v>
+        <v>113</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q10" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="R10" s="1">
+      <c r="Q10" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S10" t="s">
+      <c r="R10" t="s">
         <v>105</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X10" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="Y10" s="1" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB10" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="AC10" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="AD10" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE10" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI10" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>180</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K11" s="1">
+        <v>2018</v>
+      </c>
       <c r="L11" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M11" s="1">
         <v>5</v>
       </c>
+      <c r="M11" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N11" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>181</v>
+        <v>107</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q11" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="R11" s="1">
+      <c r="Q11" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S11" t="s">
+      <c r="R11" t="s">
         <v>70</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="S11" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="V11" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X11" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="Y11" s="1" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AB11" s="1">
+      <c r="AA11" s="1">
         <v>35801</v>
       </c>
+      <c r="AC11" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="AD11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE11" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF11" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI11" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>180</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K12" s="1">
+        <v>2018</v>
+      </c>
       <c r="L12" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M12" s="1">
         <v>5</v>
       </c>
+      <c r="M12" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N12" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>181</v>
+        <v>111</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q12" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="R12" s="1">
+      <c r="Q12" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S12" t="s">
+      <c r="R12" t="s">
         <v>115</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X12" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="Y12" s="1" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AB12" s="1">
+      <c r="AA12" s="1">
         <v>35801</v>
       </c>
+      <c r="AC12" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="AD12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE12" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF12" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI12" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K13" s="1">
+        <v>2018</v>
+      </c>
       <c r="L13" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M13" s="1">
         <v>5</v>
       </c>
+      <c r="M13" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N13" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>181</v>
+        <v>117</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q13" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="R13" s="1">
+      <c r="Q13" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S13" t="s">
+      <c r="R13" t="s">
         <v>71</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="W13" s="1" t="s">
+      <c r="V13" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X13" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="Y13" s="1" t="s">
-        <v>119</v>
+        <v>43</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA13" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="AC13" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="AD13" s="1" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="AE13" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF13" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="AG13" s="1" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="AH13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI13" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K14" s="1">
+        <v>2018</v>
+      </c>
       <c r="L14" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M14" s="1">
         <v>5</v>
       </c>
+      <c r="M14" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N14" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>181</v>
+        <v>121</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q14" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="R14" s="1">
+      <c r="Q14" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S14" t="s">
+      <c r="R14" t="s">
         <v>123</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="W14" s="1" t="s">
+      <c r="V14" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X14" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="Y14" s="1" t="s">
-        <v>130</v>
+        <v>43</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA14" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="AC14" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="AD14" s="1" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="AE14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF14" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="AG14" s="1" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="AH14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI14" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I15" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K15" s="1">
+        <v>2018</v>
+      </c>
       <c r="L15" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M15" s="1">
         <v>5</v>
       </c>
+      <c r="M15" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N15" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q15" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="R15" s="1">
+      <c r="Q15" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S15" t="s">
+      <c r="R15" t="s">
         <v>72</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="W15" s="1" t="s">
+      <c r="V15" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X15" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="Y15" s="1" t="s">
-        <v>124</v>
+        <v>43</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB15" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="AC15" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="AD15" s="1" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="AE15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF15" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="AG15" s="1" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="AH15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI15" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G16" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I16" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K16" s="1">
+        <v>2018</v>
+      </c>
       <c r="L16" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M16" s="1">
         <v>5</v>
       </c>
+      <c r="M16" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N16" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>181</v>
+        <v>133</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q16" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="R16" s="1">
+      <c r="Q16" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S16" t="s">
+      <c r="R16" t="s">
         <v>134</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="W16" s="1" t="s">
+      <c r="V16" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X16" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="Y16" s="1" t="s">
-        <v>135</v>
+        <v>43</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA16" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="AC16" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="AD16" s="1" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="AE16" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF16" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="AG16" s="1" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="AH16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI16" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G17" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I17" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K17" s="1">
+        <v>2018</v>
+      </c>
       <c r="L17" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M17" s="1">
         <v>5</v>
       </c>
+      <c r="M17" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N17" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q17" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="R17" s="1">
+      <c r="Q17" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S17" t="s">
+      <c r="R17" t="s">
         <v>73</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="W17" s="1" t="s">
+      <c r="V17" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X17" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="Y17" s="1" t="s">
-        <v>129</v>
+        <v>43</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB17" s="1" t="s">
         <v>136</v>
       </c>
+      <c r="AC17" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="AD17" s="1" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="AE17" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF17" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="AG17" s="1" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="AH17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI17" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G18" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I18" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K18" s="1">
+        <v>2018</v>
+      </c>
       <c r="L18" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M18" s="1">
         <v>5</v>
       </c>
+      <c r="M18" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N18" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>181</v>
+        <v>137</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q18" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="R18" s="1">
+      <c r="Q18" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S18" t="s">
+      <c r="R18" t="s">
         <v>74</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="V18" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X18" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="Y18" s="1" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA18" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="AC18" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="AD18" s="1" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="AE18" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF18" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="AG18" s="1" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="AH18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI18" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G19" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="K19" s="1">
+        <v>2018</v>
+      </c>
       <c r="L19" s="1">
-        <v>2018</v>
-      </c>
-      <c r="M19" s="1">
         <v>5</v>
       </c>
+      <c r="M19" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="N19" s="1" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>181</v>
+        <v>140</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q19" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="R19" s="1">
+      <c r="Q19" s="1">
         <v>15044466025</v>
       </c>
-      <c r="S19" t="s">
+      <c r="R19" t="s">
         <v>75</v>
       </c>
-      <c r="T19" s="1" t="s">
+      <c r="S19" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="W19" s="1" t="s">
+      <c r="V19" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X19" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="Y19" s="1" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB19" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="AC19" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="AD19" s="1" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="AE19" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R20" t="s">
+        <v>337</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="AD20" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AE20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AG19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH19" s="1" t="s">
+      <c r="AF20" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="AG20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AI19" s="1" t="s">
-        <v>87</v>
+      <c r="AH20" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R21" t="s">
+        <v>350</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AG21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH21" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R22" t="s">
+        <v>360</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="AD22" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF22" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R23" t="s">
+        <v>372</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AC23" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="AD23" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF23" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="AG23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH23" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R24" t="s">
+        <v>384</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AC24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD24" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF24" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="AG24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH24" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R25" t="s">
+        <v>398</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB25" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AC25" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="AD25" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="AE25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF25" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AG25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH25" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R26" t="s">
+        <v>403</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB26" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AC26" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="AD26" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="AE26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF26" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="AG26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH26" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="N27" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R27" t="s">
+        <v>407</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB27" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AC27" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="AD27" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="AE27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF27" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="AG27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH27" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R28" t="s">
+        <v>417</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB28" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AC28" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="AD28" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="AE28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF28" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="AG28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH28" s="1" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -5239,7 +6065,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P12" sqref="P12"/>
+      <selection pane="topRight" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5404,7 +6230,7 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>252</v>
+        <v>332</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>236</v>
@@ -5484,7 +6310,7 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>252</v>
+        <v>332</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>236</v>
@@ -5564,7 +6390,7 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>252</v>
+        <v>332</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>236</v>
@@ -5644,7 +6470,7 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>252</v>
+        <v>332</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>236</v>
@@ -5724,7 +6550,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>252</v>
+        <v>332</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>236</v>
@@ -5804,7 +6630,7 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>252</v>
+        <v>332</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>236</v>
@@ -5884,7 +6710,7 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>252</v>
+        <v>332</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>236</v>
@@ -5964,7 +6790,7 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>252</v>
+        <v>332</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>236</v>
@@ -6044,7 +6870,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>252</v>
+        <v>332</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>236</v>
@@ -6124,7 +6950,7 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>252</v>
+        <v>332</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>236</v>

</xml_diff>

<commit_message>
Added test for customer-facing, booking tickets with valid promo code.
</commit_message>
<xml_diff>
--- a/data/tickets.xlsx
+++ b/data/tickets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Successful" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,34 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Автор</author>
+  </authors>
+  <commentList>
+    <comment ref="S21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Автор:
+Until 01.01.2019</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="513">
   <si>
     <t>id_testdata</t>
   </si>
@@ -770,15 +796,9 @@
     <t>GoDo-710</t>
   </si>
   <si>
-    <t>GHO0001_NNCU1SC</t>
-  </si>
-  <si>
     <t>27</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>Ryan</t>
   </si>
   <si>
@@ -1275,13 +1295,301 @@
   </si>
   <si>
     <t>10:20 AM AT</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>godo-701@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-702@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-703@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-704@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-705@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-706@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-707@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-708@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-709@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-710@mailinator.com</t>
+  </si>
+  <si>
+    <t>GoDo-153</t>
+  </si>
+  <si>
+    <t>godo-153@mailinator.com</t>
+  </si>
+  <si>
+    <t>33917</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Phillips</t>
+  </si>
+  <si>
+    <t>COOL013</t>
+  </si>
+  <si>
+    <t>214.60</t>
+  </si>
+  <si>
+    <t>200.00</t>
+  </si>
+  <si>
+    <t>11.10</t>
+  </si>
+  <si>
+    <t>-15.00</t>
+  </si>
+  <si>
+    <t>18.50</t>
+  </si>
+  <si>
+    <t>GoDo-142</t>
+  </si>
+  <si>
+    <t>godo-142@mailinator.com</t>
+  </si>
+  <si>
+    <t>ANZHELA</t>
+  </si>
+  <si>
+    <t>-10.00</t>
+  </si>
+  <si>
+    <t>9.00</t>
+  </si>
+  <si>
+    <t>5.40</t>
+  </si>
+  <si>
+    <t>18951</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>104.40</t>
+  </si>
+  <si>
+    <t>GoDo-146</t>
+  </si>
+  <si>
+    <t>JULY2017</t>
+  </si>
+  <si>
+    <t>godo-146@mailinator.com</t>
+  </si>
+  <si>
+    <t>-12.00</t>
+  </si>
+  <si>
+    <t>102.08</t>
+  </si>
+  <si>
+    <t>5.28</t>
+  </si>
+  <si>
+    <t>8.80</t>
+  </si>
+  <si>
+    <t>36605</t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t>Bennett</t>
+  </si>
+  <si>
+    <t>GoDo-149</t>
+  </si>
+  <si>
+    <t>SUPER013</t>
+  </si>
+  <si>
+    <t>godo-149@mailinator.com</t>
+  </si>
+  <si>
+    <t>21801</t>
+  </si>
+  <si>
+    <t>Flores</t>
+  </si>
+  <si>
+    <t>GoDo-151</t>
+  </si>
+  <si>
+    <t>godo-151@mailinator.com</t>
+  </si>
+  <si>
+    <t>DURATIONREGR</t>
+  </si>
+  <si>
+    <t>46304</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Barnes</t>
+  </si>
+  <si>
+    <t>GoDo-155</t>
+  </si>
+  <si>
+    <t>godo-155@mailinator.com</t>
+  </si>
+  <si>
+    <t>Rebecca</t>
+  </si>
+  <si>
+    <t>Sanders</t>
+  </si>
+  <si>
+    <t>95008</t>
+  </si>
+  <si>
+    <t>300.00</t>
+  </si>
+  <si>
+    <t>330.60</t>
+  </si>
+  <si>
+    <t>28.50</t>
+  </si>
+  <si>
+    <t>17.10</t>
+  </si>
+  <si>
+    <t>GoDo-156</t>
+  </si>
+  <si>
+    <t>MAX013</t>
+  </si>
+  <si>
+    <t>godo-156@mailinator.com</t>
+  </si>
+  <si>
+    <t>Keith</t>
+  </si>
+  <si>
+    <t>53402</t>
+  </si>
+  <si>
+    <t>208.80</t>
+  </si>
+  <si>
+    <t>-20.00</t>
+  </si>
+  <si>
+    <t>18.00</t>
+  </si>
+  <si>
+    <t>10.80</t>
+  </si>
+  <si>
+    <t>GoDo-157</t>
+  </si>
+  <si>
+    <t>godo-157@mailinator.com</t>
+  </si>
+  <si>
+    <t>Catherine</t>
+  </si>
+  <si>
+    <t>Henderson</t>
+  </si>
+  <si>
+    <t>04401</t>
+  </si>
+  <si>
+    <t>92.80</t>
+  </si>
+  <si>
+    <t>8.00</t>
+  </si>
+  <si>
+    <t>4.80</t>
+  </si>
+  <si>
+    <t>GoDo-159</t>
+  </si>
+  <si>
+    <t>https://dev.godo.io/customer_facing.aspx?Activity=d7d33c05-93ea-4000-9033-80c8d2bbe006</t>
+  </si>
+  <si>
+    <t>iPad activity</t>
+  </si>
+  <si>
+    <t>07:00 AM</t>
+  </si>
+  <si>
+    <t>Bonnie</t>
+  </si>
+  <si>
+    <t>Cox</t>
+  </si>
+  <si>
+    <t>godo-159@mailinator.com</t>
+  </si>
+  <si>
+    <t>01902</t>
+  </si>
+  <si>
+    <t>MINIMUMPRICE</t>
+  </si>
+  <si>
+    <t>60.00</t>
+  </si>
+  <si>
+    <t>GoDo-312</t>
+  </si>
+  <si>
+    <t>60.01</t>
+  </si>
+  <si>
+    <t>senior</t>
+  </si>
+  <si>
+    <t>Lillian</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>godo-312@mailinator.com</t>
+  </si>
+  <si>
+    <t>06051</t>
+  </si>
+  <si>
+    <t>55.51</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1297,6 +1605,14 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1647,9 +1963,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N19" sqref="N19"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,7 +2111,7 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>35</v>
@@ -1816,31 +2132,31 @@
         <v>182</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="Q2" s="1">
         <v>15044466025</v>
       </c>
       <c r="R2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="S2" s="1">
         <v>35801</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AC2" s="1" t="s">
         <v>45</v>
@@ -1863,7 +2179,7 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>35</v>
@@ -1884,28 +2200,28 @@
         <v>182</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="Q3" s="1">
         <v>15044466025</v>
       </c>
       <c r="R3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="S3" s="1">
         <v>35801</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AC3" s="1" t="s">
         <v>45</v>
@@ -1949,10 +2265,10 @@
         <v>182</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>63</v>
@@ -2026,10 +2342,10 @@
         <v>5</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>38</v>
@@ -2103,10 +2419,10 @@
         <v>5</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>91</v>
@@ -2180,10 +2496,10 @@
         <v>5</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>94</v>
@@ -2254,10 +2570,10 @@
         <v>5</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>97</v>
@@ -2331,10 +2647,10 @@
         <v>5</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>100</v>
@@ -2408,10 +2724,10 @@
         <v>5</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>113</v>
@@ -2485,10 +2801,10 @@
         <v>5</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>107</v>
@@ -2562,10 +2878,10 @@
         <v>5</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>111</v>
@@ -2639,10 +2955,10 @@
         <v>5</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>117</v>
@@ -2713,10 +3029,10 @@
         <v>5</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>121</v>
@@ -2787,10 +3103,10 @@
         <v>5</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>125</v>
@@ -2864,10 +3180,10 @@
         <v>5</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>133</v>
@@ -2938,10 +3254,10 @@
         <v>5</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>127</v>
@@ -3015,10 +3331,10 @@
         <v>5</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>137</v>
@@ -3089,10 +3405,10 @@
         <v>5</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>140</v>
@@ -3145,614 +3461,614 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>234</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>235</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q20" s="1">
         <v>15044466025</v>
       </c>
       <c r="R20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>85</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="AD20" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="AE20" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF20" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AG20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH20" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>234</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>235</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="Q21" s="1">
         <v>15044466025</v>
       </c>
       <c r="R21" t="s">
+        <v>348</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="AC21" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="S21" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>352</v>
-      </c>
       <c r="AD21" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="AE21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF21" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AG21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH21" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>357</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>235</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="Q22" s="1">
         <v>15044466025</v>
       </c>
       <c r="R22" t="s">
+        <v>358</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="T22" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="S22" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="T22" s="1" t="s">
+      <c r="V22" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AC22" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="V22" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="AB22" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="AC22" s="1" t="s">
-        <v>364</v>
-      </c>
       <c r="AD22" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AE22" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF22" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AG22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH22" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>235</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="Q23" s="1">
         <v>15044466025</v>
       </c>
       <c r="R23" t="s">
+        <v>370</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AC23" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="AD23" s="1" t="s">
         <v>373</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="AB23" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="AC23" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="AD23" s="1" t="s">
-        <v>375</v>
       </c>
       <c r="AE23" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF23" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AG23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH23" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>36</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="N24" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="P24" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>383</v>
       </c>
       <c r="Q24" s="1">
         <v>15044466025</v>
       </c>
       <c r="R24" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AC24" s="1" t="s">
         <v>89</v>
       </c>
       <c r="AD24" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="AE24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF24" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="AG24" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH24" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q25" s="1">
         <v>15044466025</v>
       </c>
       <c r="R25" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AC25" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="AD25" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="AE25" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF25" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="AG25" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH25" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>235</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Q26" s="1">
         <v>15044466025</v>
       </c>
       <c r="R26" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="T26" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="AB26" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AC26" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="V26" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="AB26" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="AC26" s="1" t="s">
-        <v>364</v>
-      </c>
       <c r="AD26" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AE26" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF26" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AG26" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH26" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>235</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="Q27" s="1">
         <v>15044466025</v>
       </c>
       <c r="R27" t="s">
+        <v>405</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="T27" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="S27" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>409</v>
-      </c>
       <c r="V27" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AB27" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AC27" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AD27" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AE27" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF27" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AG27" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH27" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>235</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>61</v>
       </c>
       <c r="M28" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="N28" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>415</v>
-      </c>
       <c r="P28" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="Q28" s="1">
         <v>15044466025</v>
       </c>
       <c r="R28" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="V28" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AB28" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AC28" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AD28" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AE28" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF28" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AG28" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH28" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -3946,16 +4262,16 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="R2" s="1">
         <v>15044466025</v>
@@ -4029,16 +4345,16 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="R3" s="1">
         <v>15044466025</v>
@@ -4112,16 +4428,16 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="R4" s="1">
         <v>15044466025</v>
@@ -4195,16 +4511,16 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="R5" s="1">
         <v>15044466025</v>
@@ -4278,16 +4594,16 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="R6" s="1">
         <v>15044466025</v>
@@ -4361,16 +4677,16 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="R7" s="1">
         <v>15044466025</v>
@@ -4444,16 +4760,16 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="R8" s="1">
         <v>15044466025</v>
@@ -4527,16 +4843,16 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="R9" s="1">
         <v>15044466025</v>
@@ -4610,16 +4926,16 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="R10" s="1">
         <v>15044466025</v>
@@ -4693,16 +5009,16 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>181</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="R11" s="1">
         <v>15044466025</v>
@@ -4775,12 +5091,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H23" sqref="A23:H24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD28" sqref="AD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4788,29 +5104,31 @@
     <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="41.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="13.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="38.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="20" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" style="1" customWidth="1"/>
+    <col min="4" max="6" width="19.140625" style="1" customWidth="1"/>
+    <col min="7" max="9" width="22.42578125" style="1" customWidth="1"/>
+    <col min="10" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="13.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="20.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="38.28515625" style="1" customWidth="1"/>
     <col min="18" max="18" width="12.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11" style="1" customWidth="1"/>
-    <col min="20" max="20" width="13.28515625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="15" style="1" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="1"/>
+    <col min="19" max="19" width="18.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="20.42578125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="20" style="1" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="11" style="1" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="10.5703125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15" style="1" customWidth="1"/>
+    <col min="30" max="30" width="15.42578125" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4824,67 +5142,85 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="S1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>204</v>
       </c>
@@ -4897,68 +5233,68 @@
       <c r="D2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F2" s="1">
+      <c r="J2" s="1">
         <v>2018</v>
       </c>
-      <c r="G2" s="1">
+      <c r="K2" s="1">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="L2" s="1">
+      <c r="O2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="P2" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>188</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>205</v>
       </c>
@@ -4971,68 +5307,68 @@
       <c r="D3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F3" s="1">
+      <c r="J3" s="1">
         <v>2018</v>
       </c>
-      <c r="G3" s="1">
+      <c r="K3" s="1">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="L3" s="1">
+      <c r="N3" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="P3" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M3" t="s">
+      <c r="Q3" t="s">
         <v>189</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>206</v>
       </c>
@@ -5045,68 +5381,68 @@
       <c r="D4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F4" s="1">
+      <c r="J4" s="1">
         <v>2018</v>
       </c>
-      <c r="G4" s="1">
+      <c r="K4" s="1">
         <v>5</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="L4" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="L4" s="1">
+      <c r="N4" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="P4" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
         <v>190</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="1">
+      <c r="Y4" s="1">
         <v>35801</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>207</v>
       </c>
@@ -5119,68 +5455,68 @@
       <c r="D5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F5" s="1">
+      <c r="J5" s="1">
         <v>2018</v>
       </c>
-      <c r="G5" s="1">
+      <c r="K5" s="1">
         <v>5</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="L5" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="L5" s="1">
+      <c r="N5" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="P5" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M5" t="s">
+      <c r="Q5" t="s">
         <v>191</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S5" s="1">
+      <c r="Y5" s="1">
         <v>35801</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="Z5" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="AC5" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="AD5" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>208</v>
       </c>
@@ -5193,65 +5529,65 @@
       <c r="D6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F6" s="1">
+      <c r="J6" s="1">
         <v>2018</v>
       </c>
-      <c r="G6" s="1">
+      <c r="K6" s="1">
         <v>5</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="L6" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="L6" s="1">
+      <c r="N6" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="P6" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M6" t="s">
+      <c r="Q6" t="s">
         <v>192</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="AA6" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="AC6" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="AD6" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>209</v>
       </c>
@@ -5264,65 +5600,65 @@
       <c r="D7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F7" s="1">
+      <c r="J7" s="1">
         <v>2018</v>
       </c>
-      <c r="G7" s="1">
+      <c r="K7" s="1">
         <v>5</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="L7" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="L7" s="1">
+      <c r="N7" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="P7" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M7" t="s">
+      <c r="Q7" t="s">
         <v>193</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="Z7" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="AA7" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="AD7" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>210</v>
       </c>
@@ -5335,68 +5671,68 @@
       <c r="D8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F8" s="1">
+      <c r="J8" s="1">
         <v>2018</v>
       </c>
-      <c r="G8" s="1">
+      <c r="K8" s="1">
         <v>5</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="L8" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="L8" s="1">
+      <c r="N8" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="P8" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M8" t="s">
+      <c r="Q8" t="s">
         <v>194</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="W8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="X8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="Y8" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="Z8" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="AA8" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="AB8" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="AC8" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="AD8" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>211</v>
       </c>
@@ -5409,65 +5745,65 @@
       <c r="D9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F9" s="1">
+      <c r="J9" s="1">
         <v>2018</v>
       </c>
-      <c r="G9" s="1">
+      <c r="K9" s="1">
         <v>5</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="L9" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="L9" s="1">
+      <c r="P9" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M9" t="s">
+      <c r="Q9" t="s">
         <v>195</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="W9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="X9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="Z9" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="AA9" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="AB9" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="AC9" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X9" s="1" t="s">
+      <c r="AD9" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>212</v>
       </c>
@@ -5480,68 +5816,68 @@
       <c r="D10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F10" s="1">
+      <c r="J10" s="1">
         <v>2018</v>
       </c>
-      <c r="G10" s="1">
+      <c r="K10" s="1">
         <v>5</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="L10" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="L10" s="1">
+      <c r="N10" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="P10" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M10" t="s">
+      <c r="Q10" t="s">
         <v>196</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="Y10" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="Z10" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="AA10" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="AB10" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="AC10" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="AD10" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>213</v>
       </c>
@@ -5554,65 +5890,65 @@
       <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F11" s="1">
+      <c r="J11" s="1">
         <v>2018</v>
       </c>
-      <c r="G11" s="1">
+      <c r="K11" s="1">
         <v>5</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="L11" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="L11" s="1">
+      <c r="N11" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="P11" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M11" t="s">
+      <c r="Q11" t="s">
         <v>197</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="U11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="V11" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="W11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="X11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="Z11" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="AA11" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="AC11" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X11" s="1" t="s">
+      <c r="AD11" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>214</v>
       </c>
@@ -5625,68 +5961,68 @@
       <c r="D12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F12" s="1">
+      <c r="J12" s="1">
         <v>2018</v>
       </c>
-      <c r="G12" s="1">
+      <c r="K12" s="1">
         <v>5</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="L12" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L12" s="1">
+      <c r="N12" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="P12" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M12" t="s">
+      <c r="Q12" t="s">
         <v>198</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="U12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="W12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="X12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="Y12" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="Z12" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="AA12" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="AB12" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="AC12" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X12" s="1" t="s">
+      <c r="AD12" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>199</v>
       </c>
@@ -5699,68 +6035,68 @@
       <c r="D13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F13" s="1">
+      <c r="J13" s="1">
         <v>2018</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="L13" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="L13" s="1">
+      <c r="N13" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="P13" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M13" t="s">
+      <c r="Q13" t="s">
         <v>183</v>
       </c>
-      <c r="N13" s="1">
+      <c r="R13" s="1">
         <v>35801</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="U13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="V13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="W13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="X13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S13" s="1">
+      <c r="Y13" s="1">
         <v>35801</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="Z13" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U13" s="1" t="s">
+      <c r="AA13" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="AB13" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W13" s="1" t="s">
+      <c r="AC13" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X13" s="1" t="s">
+      <c r="AD13" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>200</v>
       </c>
@@ -5773,68 +6109,68 @@
       <c r="D14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F14" s="1">
+      <c r="J14" s="1">
         <v>2018</v>
       </c>
-      <c r="G14" s="1">
+      <c r="K14" s="1">
         <v>5</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="L14" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="L14" s="1">
+      <c r="N14" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="P14" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M14" t="s">
+      <c r="Q14" t="s">
         <v>184</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="U14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="V14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="W14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="Y14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="Z14" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U14" s="1" t="s">
+      <c r="AA14" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="AB14" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W14" s="1" t="s">
+      <c r="AC14" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X14" s="1" t="s">
+      <c r="AD14" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>201</v>
       </c>
@@ -5847,68 +6183,68 @@
       <c r="D15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F15" s="1">
+      <c r="J15" s="1">
         <v>2018</v>
       </c>
-      <c r="G15" s="1">
+      <c r="K15" s="1">
         <v>5</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="L15" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="L15" s="1">
+      <c r="N15" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="P15" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M15" t="s">
+      <c r="Q15" t="s">
         <v>185</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="U15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="V15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="W15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="X15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S15" s="1" t="s">
+      <c r="Y15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="Z15" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U15" s="1" t="s">
+      <c r="AA15" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="AB15" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W15" s="1" t="s">
+      <c r="AC15" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X15" s="1" t="s">
+      <c r="AD15" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>202</v>
       </c>
@@ -5921,65 +6257,65 @@
       <c r="D16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F16" s="1">
+      <c r="J16" s="1">
         <v>2018</v>
       </c>
-      <c r="G16" s="1">
+      <c r="K16" s="1">
         <v>5</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="L16" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="L16" s="1">
+      <c r="N16" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="P16" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M16" t="s">
+      <c r="Q16" t="s">
         <v>186</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="U16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="V16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="W16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="X16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="Z16" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U16" s="1" t="s">
+      <c r="AA16" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V16" s="1" t="s">
+      <c r="AB16" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W16" s="1" t="s">
+      <c r="AC16" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X16" s="1" t="s">
+      <c r="AD16" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>203</v>
       </c>
@@ -5992,70 +6328,844 @@
       <c r="D17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="1">
+      <c r="J17" s="1">
         <v>2018</v>
       </c>
-      <c r="G17" s="1">
+      <c r="K17" s="1">
         <v>5</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I17" s="1" t="s">
+      <c r="L17" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="L17" s="1">
+      <c r="N17" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="P17" s="1">
         <v>15044466025</v>
       </c>
-      <c r="M17" t="s">
+      <c r="Q17" t="s">
         <v>187</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="U17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="V17" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="W17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="X17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="Y17" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="Z17" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="AA17" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="AB17" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="W17" s="1" t="s">
+      <c r="AC17" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="AD17" s="1" t="s">
         <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K18" s="1">
+        <v>5</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="P18" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>440</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K19" s="1">
+        <v>5</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="P19" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>450</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD19" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J20" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K20" s="1">
+        <v>5</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="P20" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>460</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="AD20" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J21" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K21" s="1">
+        <v>5</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="P21" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>464</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J22" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K22" s="1">
+        <v>5</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="P22" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>429</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="AD22" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J23" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K23" s="1">
+        <v>5</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="P23" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>470</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="AC23" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="AD23" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J24" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K24" s="1">
+        <v>5</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="P24" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>480</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="AC24" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="AD24" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J25" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K25" s="1">
+        <v>5</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="P25" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>488</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="AB25" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="AC25" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="AD25" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="J26" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K26" s="1">
+        <v>5</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="P26" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>501</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="AA26" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="AB26" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC26" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD26" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="J27" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K27" s="1">
+        <v>5</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="P27" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>510</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AA27" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="AB27" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC27" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD27" s="1" t="s">
+        <v>512</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="AC18" twoDigitTextYear="1"/>
+  </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6064,8 +7174,8 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N15" sqref="N15"/>
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6230,28 +7340,25 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>332</v>
+        <v>417</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="R2" s="1">
         <v>15044466025</v>
       </c>
       <c r="S2" t="s">
-        <v>150</v>
+        <v>418</v>
       </c>
       <c r="T2" s="1">
         <v>35801</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>41</v>
@@ -6310,28 +7417,25 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>332</v>
+        <v>417</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="R3" s="1">
         <v>15044466025</v>
       </c>
       <c r="S3" t="s">
-        <v>151</v>
+        <v>419</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>41</v>
@@ -6390,28 +7494,25 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>332</v>
+        <v>417</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="R4" s="1">
         <v>15044466025</v>
       </c>
       <c r="S4" t="s">
-        <v>152</v>
+        <v>420</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>41</v>
@@ -6470,28 +7571,25 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>332</v>
+        <v>417</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="R5" s="1">
         <v>15044466025</v>
       </c>
       <c r="S5" t="s">
-        <v>153</v>
+        <v>421</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>41</v>
@@ -6550,28 +7648,25 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>332</v>
+        <v>417</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="R6" s="1">
         <v>15044466025</v>
       </c>
       <c r="S6" t="s">
-        <v>154</v>
+        <v>422</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>41</v>
@@ -6630,28 +7725,25 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>332</v>
+        <v>417</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="R7" s="1">
         <v>15044466025</v>
       </c>
       <c r="S7" t="s">
-        <v>166</v>
+        <v>423</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>41</v>
@@ -6710,28 +7802,25 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>332</v>
+        <v>417</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="R8" s="1">
         <v>15044466025</v>
       </c>
       <c r="S8" t="s">
-        <v>178</v>
+        <v>424</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="W8" s="1" t="s">
         <v>41</v>
@@ -6790,28 +7879,25 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>332</v>
+        <v>417</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="R9" s="1">
         <v>15044466025</v>
       </c>
       <c r="S9" t="s">
-        <v>177</v>
+        <v>425</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>41</v>
@@ -6870,28 +7956,25 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>332</v>
+        <v>417</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="R10" s="1">
         <v>15044466025</v>
       </c>
       <c r="S10" t="s">
-        <v>177</v>
+        <v>426</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>41</v>
@@ -6950,28 +8033,25 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>332</v>
+        <v>417</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>236</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="R11" s="1">
         <v>15044466025</v>
       </c>
       <c r="S11" t="s">
-        <v>179</v>
+        <v>427</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Added test for customer-facing, booking tickets with invalid promo code.
</commit_message>
<xml_diff>
--- a/data/tickets.xlsx
+++ b/data/tickets.xlsx
@@ -39,12 +39,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="J30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Автор:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+There is no event on su and sa.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2179" uniqueCount="557">
   <si>
     <t>id_testdata</t>
   </si>
@@ -1583,13 +1609,145 @@
   </si>
   <si>
     <t>55.51</t>
+  </si>
+  <si>
+    <t>GoDo-147</t>
+  </si>
+  <si>
+    <t>godo-147@mailinator.com</t>
+  </si>
+  <si>
+    <t>Walton</t>
+  </si>
+  <si>
+    <t>98503</t>
+  </si>
+  <si>
+    <t>72OFF</t>
+  </si>
+  <si>
+    <t>12.00</t>
+  </si>
+  <si>
+    <t>232.00</t>
+  </si>
+  <si>
+    <t>GoDo-148</t>
+  </si>
+  <si>
+    <t>Ruth</t>
+  </si>
+  <si>
+    <t>Gutierrez</t>
+  </si>
+  <si>
+    <t>godo-148@mailinator.com</t>
+  </si>
+  <si>
+    <t>07076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NICE2017 </t>
+  </si>
+  <si>
+    <t>30.00</t>
+  </si>
+  <si>
+    <t>348.00</t>
+  </si>
+  <si>
+    <t>GoDo-150</t>
+  </si>
+  <si>
+    <t>https://dev.godo.io/customer_facing.aspx?Activity=02a8b72d-d57b-4c3e-88ab-2aecf83d7b92</t>
+  </si>
+  <si>
+    <t>activity07-013</t>
+  </si>
+  <si>
+    <t>01:00 PM</t>
+  </si>
+  <si>
+    <t>Massey</t>
+  </si>
+  <si>
+    <t>godo-150@mailinator.com</t>
+  </si>
+  <si>
+    <t>06512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUPER013 </t>
+  </si>
+  <si>
+    <t>0.30</t>
+  </si>
+  <si>
+    <t>5.30</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>11:30 AM</t>
+  </si>
+  <si>
+    <t>GoDo-152</t>
+  </si>
+  <si>
+    <t>godo-152@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXPIRED013 </t>
+  </si>
+  <si>
+    <t>92806</t>
+  </si>
+  <si>
+    <t>Tina</t>
+  </si>
+  <si>
+    <t>Roberts</t>
+  </si>
+  <si>
+    <t>GoDo-154</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Robinson</t>
+  </si>
+  <si>
+    <t>godo-154@mailinator.com</t>
+  </si>
+  <si>
+    <t>46322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COOL013 </t>
+  </si>
+  <si>
+    <t>GoDo-158</t>
+  </si>
+  <si>
+    <t>godo-158@mailinator.com</t>
+  </si>
+  <si>
+    <t>Debra</t>
+  </si>
+  <si>
+    <t>Cook</t>
+  </si>
+  <si>
+    <t>27405</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1605,6 +1763,13 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
@@ -5092,11 +5257,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD27"/>
+  <dimension ref="A1:AD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD28" sqref="AD28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5610,10 +5775,10 @@
         <v>5</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>280</v>
@@ -5681,10 +5846,10 @@
         <v>5</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>282</v>
@@ -5755,10 +5920,10 @@
         <v>5</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>133</v>
@@ -5826,10 +5991,10 @@
         <v>5</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>284</v>
@@ -5900,10 +6065,10 @@
         <v>5</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>286</v>
@@ -5971,10 +6136,10 @@
         <v>5</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>288</v>
@@ -6045,10 +6210,10 @@
         <v>182</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>290</v>
@@ -6119,10 +6284,10 @@
         <v>5</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>292</v>
@@ -6193,10 +6358,10 @@
         <v>5</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>294</v>
@@ -6267,10 +6432,10 @@
         <v>5</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>296</v>
@@ -6338,10 +6503,10 @@
         <v>5</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>298</v>
@@ -6412,10 +6577,10 @@
         <v>5</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>446</v>
@@ -6489,10 +6654,10 @@
         <v>5</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>456</v>
@@ -6566,10 +6731,10 @@
         <v>5</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>380</v>
@@ -6643,10 +6808,10 @@
         <v>5</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>467</v>
@@ -6720,10 +6885,10 @@
         <v>5</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>431</v>
@@ -6797,10 +6962,10 @@
         <v>5</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>471</v>
@@ -6874,10 +7039,10 @@
         <v>5</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>481</v>
@@ -6951,10 +7116,10 @@
         <v>5</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>417</v>
+        <v>538</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>489</v>
@@ -7012,7 +7177,7 @@
       <c r="B26" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="5" t="s">
         <v>497</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -7089,7 +7254,7 @@
       <c r="B27" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="5" t="s">
         <v>497</v>
       </c>
       <c r="F27" s="1" t="s">
@@ -7157,6 +7322,360 @@
       </c>
       <c r="AD27" s="1" t="s">
         <v>512</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J28" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K28" s="1">
+        <v>5</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="P28" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>514</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="Z28" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="AB28" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC28" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="AD28" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J29" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K29" s="1">
+        <v>5</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="P29" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>523</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="AC29" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="AD29" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="J30" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K30" s="1">
+        <v>5</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="P30" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>533</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="Z30" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC30" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="AD30" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J31" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K31" s="1">
+        <v>5</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="P31" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>541</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB31" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC31" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AD31" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J32" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K32" s="1">
+        <v>5</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="P32" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>549</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="Z32" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB32" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC32" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AD32" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J33" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K33" s="1">
+        <v>5</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="P33" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>553</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="Z33" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="AB33" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="AC33" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="AD33" s="1" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -7174,8 +7693,8 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A11" sqref="A11"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7343,7 +7862,7 @@
         <v>417</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>300</v>
@@ -7420,7 +7939,7 @@
         <v>417</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>302</v>
@@ -7497,7 +8016,7 @@
         <v>417</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>304</v>
@@ -7574,7 +8093,7 @@
         <v>417</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>306</v>
@@ -7651,7 +8170,7 @@
         <v>417</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>308</v>
@@ -7728,7 +8247,7 @@
         <v>417</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>310</v>
@@ -7805,7 +8324,7 @@
         <v>417</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>312</v>
@@ -7882,7 +8401,7 @@
         <v>417</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>314</v>
@@ -7959,7 +8478,7 @@
         <v>417</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>316</v>
@@ -8036,7 +8555,7 @@
         <v>417</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>318</v>

</xml_diff>

<commit_message>
Added test for booking via admin, applying invalid promo code.
</commit_message>
<xml_diff>
--- a/data/tickets.xlsx
+++ b/data/tickets.xlsx
@@ -18,6 +18,43 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Автор</author>
+  </authors>
+  <commentList>
+    <comment ref="K22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Автор:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+Choose any future date (up to December, 1, 2018) on the calendar.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Автор</author>
@@ -70,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2179" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2400" uniqueCount="637">
   <si>
     <t>id_testdata</t>
   </si>
@@ -1032,9 +1069,6 @@
     <t>Riley</t>
   </si>
   <si>
-    <t>GoDo-Cash +</t>
-  </si>
-  <si>
     <t>GoDo-Cash -</t>
   </si>
   <si>
@@ -1056,15 +1090,9 @@
     <t>Hutchison</t>
   </si>
   <si>
-    <t>godo-cash+@mailinator.com</t>
-  </si>
-  <si>
     <t>godo-cash-@mailinator.com</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
     <t>2:00 PM CT</t>
   </si>
   <si>
@@ -1741,6 +1769,255 @@
   </si>
   <si>
     <t>27405</t>
+  </si>
+  <si>
+    <t>GoDo-277</t>
+  </si>
+  <si>
+    <t>Janice</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>godo-277@mailinator.com</t>
+  </si>
+  <si>
+    <t>77478</t>
+  </si>
+  <si>
+    <t>57701</t>
+  </si>
+  <si>
+    <t>TAI</t>
+  </si>
+  <si>
+    <t>$100.00</t>
+  </si>
+  <si>
+    <t>$10.00</t>
+  </si>
+  <si>
+    <t>$110.00</t>
+  </si>
+  <si>
+    <t>GoDo-282</t>
+  </si>
+  <si>
+    <t>Raymond</t>
+  </si>
+  <si>
+    <t>Nelson</t>
+  </si>
+  <si>
+    <t>godo-282@mailinator.com</t>
+  </si>
+  <si>
+    <t>23112</t>
+  </si>
+  <si>
+    <t>GoDo-285</t>
+  </si>
+  <si>
+    <t>Stephanie</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>godo-285@mailinator.com</t>
+  </si>
+  <si>
+    <t>08816</t>
+  </si>
+  <si>
+    <t>$25.00</t>
+  </si>
+  <si>
+    <t>- $2.50</t>
+  </si>
+  <si>
+    <t>$2.25</t>
+  </si>
+  <si>
+    <t>$24.75</t>
+  </si>
+  <si>
+    <t>GoDo-287</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>godo-287@mailinator.com</t>
+  </si>
+  <si>
+    <t>Clarence</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>02472</t>
+  </si>
+  <si>
+    <t>286REGRESS</t>
+  </si>
+  <si>
+    <t>$105.00</t>
+  </si>
+  <si>
+    <t>$10.50</t>
+  </si>
+  <si>
+    <t>$115.50</t>
+  </si>
+  <si>
+    <t>GoDo-295</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>godo-295@mailinator.com</t>
+  </si>
+  <si>
+    <t>CASE122</t>
+  </si>
+  <si>
+    <t>Rose</t>
+  </si>
+  <si>
+    <t>55068</t>
+  </si>
+  <si>
+    <t>$55.00</t>
+  </si>
+  <si>
+    <t>$5.50</t>
+  </si>
+  <si>
+    <t>$60.50</t>
+  </si>
+  <si>
+    <t>GoDo-303</t>
+  </si>
+  <si>
+    <t>Activitytesting</t>
+  </si>
+  <si>
+    <t>7:10 PM AT</t>
+  </si>
+  <si>
+    <t>Timothy</t>
+  </si>
+  <si>
+    <t>godo-303@mailinator.com</t>
+  </si>
+  <si>
+    <t>30117</t>
+  </si>
+  <si>
+    <t>$19.99</t>
+  </si>
+  <si>
+    <t>$20.99</t>
+  </si>
+  <si>
+    <t>GoDo-304</t>
+  </si>
+  <si>
+    <t>godo-304@mailinator.com</t>
+  </si>
+  <si>
+    <t>Jacqueline</t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>01876</t>
+  </si>
+  <si>
+    <t>GoDo-307</t>
+  </si>
+  <si>
+    <t>Tammy</t>
+  </si>
+  <si>
+    <t>Ross</t>
+  </si>
+  <si>
+    <t>godo-307@mailinator.com</t>
+  </si>
+  <si>
+    <t>07424</t>
+  </si>
+  <si>
+    <t>GoDo-313</t>
+  </si>
+  <si>
+    <t>godo-313@mailinator.com</t>
+  </si>
+  <si>
+    <t>Coleman</t>
+  </si>
+  <si>
+    <t>27587</t>
+  </si>
+  <si>
+    <t>66.59</t>
+  </si>
+  <si>
+    <t>59.99</t>
+  </si>
+  <si>
+    <t>3.60</t>
+  </si>
+  <si>
+    <t>GoDo-315</t>
+  </si>
+  <si>
+    <t>godo-315@mailinator.com</t>
+  </si>
+  <si>
+    <t>27870</t>
+  </si>
+  <si>
+    <t>$1,000.00</t>
+  </si>
+  <si>
+    <t>$1,050.00</t>
+  </si>
+  <si>
+    <t>GoDo-320</t>
+  </si>
+  <si>
+    <t>tyuiop</t>
+  </si>
+  <si>
+    <t>Helen</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>godo-320@mailinator.com</t>
+  </si>
+  <si>
+    <t>17013</t>
+  </si>
+  <si>
+    <t>GoDo-321</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>godo-321@mailinator.com</t>
+  </si>
+  <si>
+    <t>32250</t>
   </si>
 </sst>
 </file>
@@ -2125,12 +2402,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1:I1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2276,20 +2555,17 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>320</v>
+        <v>622</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
+        <v>216</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>364</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="K2" s="1">
         <v>2018</v>
       </c>
@@ -2299,32 +2575,32 @@
       <c r="M2" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>331</v>
+      <c r="N2" s="4" t="s">
+        <v>358</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q2" s="1">
         <v>15044466025</v>
       </c>
       <c r="R2" t="s">
-        <v>328</v>
-      </c>
-      <c r="S2" s="1">
-        <v>35801</v>
+        <v>623</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>624</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>45</v>
+        <v>625</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>46</v>
@@ -2333,18 +2609,18 @@
         <v>46</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>48</v>
+        <v>369</v>
       </c>
       <c r="AG2" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>50</v>
+        <v>626</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>35</v>
@@ -2368,25 +2644,25 @@
         <v>250</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="Q3" s="1">
         <v>15044466025</v>
       </c>
       <c r="R3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="S3" s="1">
         <v>35801</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AC3" s="1" t="s">
         <v>45</v>
@@ -2433,7 +2709,7 @@
         <v>250</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>63</v>
@@ -2510,7 +2786,7 @@
         <v>250</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>38</v>
@@ -2587,7 +2863,7 @@
         <v>250</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>91</v>
@@ -2664,7 +2940,7 @@
         <v>250</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>94</v>
@@ -2738,7 +3014,7 @@
         <v>250</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>97</v>
@@ -2815,7 +3091,7 @@
         <v>250</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>100</v>
@@ -2892,7 +3168,7 @@
         <v>250</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>113</v>
@@ -2969,7 +3245,7 @@
         <v>250</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>107</v>
@@ -3046,7 +3322,7 @@
         <v>250</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>111</v>
@@ -3123,7 +3399,7 @@
         <v>250</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>117</v>
@@ -3197,7 +3473,7 @@
         <v>250</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>121</v>
@@ -3271,7 +3547,7 @@
         <v>250</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>125</v>
@@ -3348,7 +3624,7 @@
         <v>250</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>133</v>
@@ -3422,7 +3698,7 @@
         <v>250</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>127</v>
@@ -3499,7 +3775,7 @@
         <v>250</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>137</v>
@@ -3573,7 +3849,7 @@
         <v>250</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>140</v>
@@ -3626,619 +3902,1229 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>234</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>235</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>330</v>
+        <v>414</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="Q20" s="1">
         <v>15044466025</v>
       </c>
       <c r="R20" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>85</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AC20" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AD20" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="AD20" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="AE20" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF20" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="AG20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH20" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>234</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>235</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>330</v>
+        <v>414</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="Q21" s="1">
         <v>15044466025</v>
       </c>
       <c r="R21" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AC21" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="AD21" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="AE21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF21" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="AG21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH21" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>353</v>
+        <v>569</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>355</v>
+        <v>182</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>235</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>330</v>
+        <v>414</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>356</v>
+        <v>570</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>357</v>
+        <v>571</v>
       </c>
       <c r="Q22" s="1">
         <v>15044466025</v>
       </c>
       <c r="R22" t="s">
-        <v>358</v>
+        <v>572</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>359</v>
+        <v>573</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="AB22" s="1" t="s">
         <v>322</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>362</v>
+        <v>574</v>
       </c>
       <c r="AD22" s="1" t="s">
-        <v>363</v>
+        <v>575</v>
       </c>
       <c r="AE22" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF22" s="1" t="s">
-        <v>364</v>
+        <v>576</v>
       </c>
       <c r="AG22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH22" s="1" t="s">
-        <v>365</v>
+        <v>577</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>235</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>330</v>
+        <v>414</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="Q23" s="1">
         <v>15044466025</v>
       </c>
       <c r="R23" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="T23" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AC23" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="AD23" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="AB23" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="AC23" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="AD23" s="1" t="s">
-        <v>373</v>
       </c>
       <c r="AE23" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF23" s="1" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="AG23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH23" s="1" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>377</v>
+        <v>351</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>36</v>
+        <v>235</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>379</v>
+        <v>414</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>358</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="Q24" s="1">
         <v>15044466025</v>
       </c>
       <c r="R24" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AC24" s="1" t="s">
-        <v>89</v>
+        <v>369</v>
       </c>
       <c r="AD24" s="1" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="AE24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF24" s="1" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="AG24" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH24" s="1" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>333</v>
+        <v>375</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>391</v>
+        <v>36</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="N25" s="5" t="s">
-        <v>389</v>
+        <v>414</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>376</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>290</v>
+        <v>378</v>
       </c>
       <c r="Q25" s="1">
         <v>15044466025</v>
       </c>
       <c r="R25" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AC25" s="1" t="s">
-        <v>392</v>
+        <v>89</v>
       </c>
       <c r="AD25" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="AE25" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF25" s="1" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="AG25" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH25" s="1" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>354</v>
+        <v>385</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>355</v>
+        <v>61</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>330</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>235</v>
+        <v>387</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>388</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>182</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>330</v>
+        <v>414</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>361</v>
+        <v>386</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>400</v>
+        <v>290</v>
       </c>
       <c r="Q26" s="1">
         <v>15044466025</v>
       </c>
       <c r="R26" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>359</v>
+        <v>392</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AB26" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AC26" s="1" t="s">
-        <v>362</v>
+        <v>389</v>
       </c>
       <c r="AD26" s="1" t="s">
-        <v>363</v>
+        <v>381</v>
       </c>
       <c r="AE26" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF26" s="1" t="s">
-        <v>364</v>
+        <v>390</v>
       </c>
       <c r="AG26" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH26" s="1" t="s">
-        <v>365</v>
+        <v>391</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="K27" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>409</v>
+      <c r="K27" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>414</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="Q27" s="1">
         <v>15044466025</v>
       </c>
       <c r="R27" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>406</v>
+        <v>356</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>407</v>
+        <v>357</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AB27" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AC27" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="AD27" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="AE27" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF27" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="AG27" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH27" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>235</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>412</v>
+        <v>335</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>61</v>
+        <v>405</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>416</v>
+        <v>358</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="Q28" s="1">
         <v>15044466025</v>
       </c>
       <c r="R28" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="V28" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AB28" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AC28" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="AD28" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="AE28" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AF28" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="AG28" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AH28" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R29" t="s">
+        <v>412</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AC29" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="AD29" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="AE29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF29" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AG29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH29" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R30" t="s">
+        <v>557</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AC30" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="AD30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF30" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="AG30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH30" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R31" t="s">
+        <v>567</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB31" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AC31" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="AD31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF31" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="AG31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH31" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R32" t="s">
+        <v>580</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB32" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AC32" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="AD32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF32" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="AG32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH32" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R33" t="s">
+        <v>590</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB33" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AC33" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="AD33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF33" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="AG33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH33" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="N34" s="5" t="s">
+        <v>599</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R34" t="s">
+        <v>601</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB34" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AC34" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="AD34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH34" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R35" t="s">
+        <v>606</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB35" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AC35" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="AD35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF35" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="AG35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH35" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R36" t="s">
+        <v>613</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB36" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AC36" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="AD36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF36" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="AG36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH36" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R37" t="s">
+        <v>631</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AC37" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="AD37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF37" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="AG37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH37" s="1" t="s">
+        <v>563</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4248,7 +5134,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q17" sqref="Q17"/>
+      <selection pane="topRight" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5257,18 +6143,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD33"/>
+  <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="6" width="19.140625" style="1" customWidth="1"/>
     <col min="7" max="9" width="22.42578125" style="1" customWidth="1"/>
     <col min="10" max="12" width="9.140625" style="1"/>
@@ -5408,7 +6296,7 @@
         <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>236</v>
@@ -5482,7 +6370,7 @@
         <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>236</v>
@@ -5556,7 +6444,7 @@
         <v>5</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>236</v>
@@ -5630,7 +6518,7 @@
         <v>5</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>236</v>
@@ -5704,7 +6592,7 @@
         <v>5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>236</v>
@@ -5775,10 +6663,10 @@
         <v>5</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>280</v>
@@ -5846,10 +6734,10 @@
         <v>5</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>282</v>
@@ -5920,10 +6808,10 @@
         <v>5</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>133</v>
@@ -5991,10 +6879,10 @@
         <v>5</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>284</v>
@@ -6065,10 +6953,10 @@
         <v>5</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>286</v>
@@ -6136,10 +7024,10 @@
         <v>5</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>288</v>
@@ -6210,10 +7098,10 @@
         <v>182</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>290</v>
@@ -6284,10 +7172,10 @@
         <v>5</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>292</v>
@@ -6358,10 +7246,10 @@
         <v>5</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>294</v>
@@ -6432,10 +7320,10 @@
         <v>5</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>296</v>
@@ -6503,10 +7391,10 @@
         <v>5</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>298</v>
@@ -6556,7 +7444,7 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>233</v>
@@ -6577,13 +7465,13 @@
         <v>5</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>267</v>
@@ -6592,13 +7480,13 @@
         <v>15044466025</v>
       </c>
       <c r="Q18" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>41</v>
@@ -6619,21 +7507,21 @@
         <v>218</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="AC18" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="AD18" s="1" t="s">
         <v>444</v>
-      </c>
-      <c r="AD18" s="1" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>233</v>
@@ -6654,28 +7542,28 @@
         <v>5</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="P19" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q19" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="U19" s="1" t="s">
         <v>41</v>
@@ -6696,21 +7584,21 @@
         <v>218</v>
       </c>
       <c r="AA19" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="AB19" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="AB19" s="1" t="s">
-        <v>454</v>
-      </c>
       <c r="AC19" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="AD19" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>233</v>
@@ -6731,28 +7619,28 @@
         <v>5</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="P20" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q20" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="U20" s="1" t="s">
         <v>41</v>
@@ -6773,21 +7661,21 @@
         <v>218</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="AC20" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="AD20" s="1" t="s">
         <v>444</v>
-      </c>
-      <c r="AD20" s="1" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>233</v>
@@ -6808,28 +7696,28 @@
         <v>5</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="P21" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q21" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="U21" s="1" t="s">
         <v>41</v>
@@ -6850,21 +7738,21 @@
         <v>218</v>
       </c>
       <c r="AA21" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="AC21" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="AD21" s="1" t="s">
         <v>444</v>
-      </c>
-      <c r="AD21" s="1" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>233</v>
@@ -6873,7 +7761,7 @@
         <v>234</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>235</v>
@@ -6885,28 +7773,28 @@
         <v>5</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="P22" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q22" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="R22" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="S22" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>433</v>
       </c>
       <c r="U22" s="1" t="s">
         <v>41</v>
@@ -6924,24 +7812,24 @@
         <v>76</v>
       </c>
       <c r="Z22" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="AB22" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="AA22" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="AB22" s="1" t="s">
-        <v>438</v>
-      </c>
       <c r="AC22" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="AD22" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>233</v>
@@ -6950,7 +7838,7 @@
         <v>234</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>235</v>
@@ -6962,28 +7850,28 @@
         <v>5</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="P23" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q23" t="s">
+        <v>467</v>
+      </c>
+      <c r="R23" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="R23" s="1" t="s">
-        <v>473</v>
-      </c>
       <c r="S23" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="U23" s="1" t="s">
         <v>41</v>
@@ -7001,24 +7889,24 @@
         <v>76</v>
       </c>
       <c r="Z23" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="AC23" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="AA23" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="AB23" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="AC23" s="1" t="s">
-        <v>477</v>
-      </c>
       <c r="AD23" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>233</v>
@@ -7027,7 +7915,7 @@
         <v>234</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>235</v>
@@ -7039,13 +7927,13 @@
         <v>5</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>285</v>
@@ -7054,13 +7942,13 @@
         <v>15044466025</v>
       </c>
       <c r="Q24" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="U24" s="1" t="s">
         <v>41</v>
@@ -7078,24 +7966,24 @@
         <v>76</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="AC24" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="AD24" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>233</v>
@@ -7116,28 +8004,28 @@
         <v>5</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="P25" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q25" t="s">
+        <v>485</v>
+      </c>
+      <c r="R25" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="R25" s="1" t="s">
-        <v>491</v>
-      </c>
       <c r="S25" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="U25" s="1" t="s">
         <v>41</v>
@@ -7158,33 +8046,33 @@
         <v>218</v>
       </c>
       <c r="AA25" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="AC25" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="AD25" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="J26" s="1">
         <v>2018</v>
@@ -7193,28 +8081,28 @@
         <v>5</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="P26" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q26" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="U26" s="1" t="s">
         <v>41</v>
@@ -7232,10 +8120,10 @@
         <v>76</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="AA26" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="AB26" s="1" t="s">
         <v>224</v>
@@ -7249,19 +8137,19 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>61</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="J27" s="1">
         <v>2018</v>
@@ -7270,28 +8158,28 @@
         <v>5</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="P27" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q27" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="U27" s="1" t="s">
         <v>41</v>
@@ -7309,10 +8197,10 @@
         <v>76</v>
       </c>
       <c r="Z27" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="AA27" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="AB27" s="1" t="s">
         <v>224</v>
@@ -7321,12 +8209,12 @@
         <v>225</v>
       </c>
       <c r="AD27" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>233</v>
@@ -7335,7 +8223,7 @@
         <v>234</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>235</v>
@@ -7347,45 +8235,45 @@
         <v>5</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>125</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="P28" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q28" t="s">
+        <v>511</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="S28" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="R28" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>517</v>
-      </c>
       <c r="Z28" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="AB28" s="1" t="s">
         <v>226</v>
       </c>
       <c r="AC28" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="AD28" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>233</v>
@@ -7394,7 +8282,7 @@
         <v>234</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>235</v>
@@ -7406,57 +8294,57 @@
         <v>5</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="P29" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q29" t="s">
+        <v>520</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB29" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="R29" s="1" t="s">
+      <c r="AC29" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="AD29" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="S29" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="Z29" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="AB29" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="AC29" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="AD29" s="1" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="J30" s="1">
         <v>2018</v>
@@ -7465,28 +8353,28 @@
         <v>5</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="P30" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q30" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="Z30" s="1" t="s">
         <v>220</v>
@@ -7495,15 +8383,15 @@
         <v>222</v>
       </c>
       <c r="AC30" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD30" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>233</v>
@@ -7524,28 +8412,28 @@
         <v>5</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="P31" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q31" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="Z31" s="1" t="s">
         <v>218</v>
@@ -7562,7 +8450,7 @@
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>233</v>
@@ -7583,28 +8471,28 @@
         <v>5</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="P32" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q32" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="Z32" s="1" t="s">
         <v>218</v>
@@ -7621,7 +8509,7 @@
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>233</v>
@@ -7630,7 +8518,7 @@
         <v>234</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>235</v>
@@ -7642,40 +8530,158 @@
         <v>5</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="P33" s="1">
         <v>15044466025</v>
       </c>
       <c r="Q33" t="s">
+        <v>550</v>
+      </c>
+      <c r="R33" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="R33" s="1" t="s">
-        <v>556</v>
-      </c>
       <c r="S33" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="Z33" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="AB33" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="AC33" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="AD33" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="J34" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K34" s="1">
+        <v>5</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="P34" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>616</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="Z34" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="AB34" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC34" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="AD34" s="1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="J35" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K35" s="1">
+        <v>5</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="P35" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>635</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="Z35" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="AB35" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC35" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="AD35" s="1" t="s">
+        <v>619</v>
       </c>
     </row>
   </sheetData>
@@ -7859,10 +8865,10 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>300</v>
@@ -7874,7 +8880,7 @@
         <v>15044466025</v>
       </c>
       <c r="S2" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="T2" s="1">
         <v>35801</v>
@@ -7936,10 +8942,10 @@
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>302</v>
@@ -7951,7 +8957,7 @@
         <v>15044466025</v>
       </c>
       <c r="S3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>76</v>
@@ -8013,10 +9019,10 @@
         <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>304</v>
@@ -8028,7 +9034,7 @@
         <v>15044466025</v>
       </c>
       <c r="S4" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>77</v>
@@ -8090,10 +9096,10 @@
         <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>306</v>
@@ -8105,7 +9111,7 @@
         <v>15044466025</v>
       </c>
       <c r="S5" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>78</v>
@@ -8167,10 +9173,10 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>308</v>
@@ -8182,7 +9188,7 @@
         <v>15044466025</v>
       </c>
       <c r="S6" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>79</v>
@@ -8244,10 +9250,10 @@
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>310</v>
@@ -8259,7 +9265,7 @@
         <v>15044466025</v>
       </c>
       <c r="S7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>80</v>
@@ -8321,10 +9327,10 @@
         <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>312</v>
@@ -8336,7 +9342,7 @@
         <v>15044466025</v>
       </c>
       <c r="S8" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>80</v>
@@ -8398,10 +9404,10 @@
         <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>314</v>
@@ -8413,7 +9419,7 @@
         <v>15044466025</v>
       </c>
       <c r="S9" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>81</v>
@@ -8475,10 +9481,10 @@
         <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>316</v>
@@ -8490,7 +9496,7 @@
         <v>15044466025</v>
       </c>
       <c r="S10" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>81</v>
@@ -8552,10 +9558,10 @@
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>318</v>
@@ -8567,7 +9573,7 @@
         <v>15044466025</v>
       </c>
       <c r="S11" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>82</v>

</xml_diff>